<commit_message>
Catch22 reordering of features
</commit_message>
<xml_diff>
--- a/tsml_eval/_wip/catch22/aeon_catch22_with_numba.xlsx
+++ b/tsml_eval/_wip/catch22/aeon_catch22_with_numba.xlsx
@@ -431,124 +431,124 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>mode_5</t>
+          <t>DN_HistogramMode_5</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>mode_10</t>
+          <t>DN_HistogramMode_10</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>stretch_high</t>
+          <t>CO_f1ecac</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>outlier_timing_pos</t>
+          <t>CO_FirstMin_ac</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>outlier_timing_neg</t>
+          <t>CO_HistogramAMI_even_2_5</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>acf_timescale</t>
+          <t>CO_trev_1_num</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>acf_first_min</t>
+          <t>MD_hrv_classic_pnn40</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>centroid_freq</t>
+          <t>SB_BinaryStats_mean_longstretch1</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>low_freq_power</t>
+          <t>SB_TransitionMatrix_3ac_sumdiagcov</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>forecast_error</t>
+          <t>PD_PeriodicityWang_th0_01</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>trev</t>
+          <t>CO_Embed2_Dist_tau_d_expfit_meandiff</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>ami2</t>
+          <t>IN_AutoMutualInfoStats_40_gaussian_fmmi</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>ami_timescale</t>
+          <t>FC_LocalSimple_mean1_tauresrat</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>high_fluctuation</t>
+          <t>DN_OutlierInclude_p_001_mdrmd</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>stretch_decreasing</t>
+          <t>DN_OutlierInclude_n_001_mdrmd</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>entropy_pairs</t>
+          <t>SP_Summaries_welch_rect_area_5_1</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>whiten_timescale</t>
+          <t>SB_BinaryStats_diff_longstretch0</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>periodicity</t>
+          <t>SB_MotifThree_quantile_hh</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>dfa</t>
+          <t>SC_FluctAnal_2_rsrangefit_50_1_logi_prop_r1</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>rs_range</t>
+          <t>SC_FluctAnal_2_dfa_50_1_2_logi_prop_r1</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>transition_matrix</t>
+          <t>SP_Summaries_welch_rect_centroid</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>periodicity</t>
+          <t>FC_LocalSimple_mean3_stderr</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.15862957</v>
+        <v>1.158629536628723</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.2172266650000001</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2.586673782144931</v>
+        <v>-0.2172266840934753</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="D2" t="n">
         <v>6</v>
@@ -562,8 +562,8 @@
       <c r="G2" t="n">
         <v>1</v>
       </c>
-      <c r="H2" t="n">
-        <v>8</v>
+      <c r="H2" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="I2" t="n">
         <v>0.04000000000000001</v>
@@ -589,11 +589,11 @@
       <c r="P2" t="n">
         <v>0.4680519470663282</v>
       </c>
-      <c r="Q2" t="n">
-        <v>5</v>
-      </c>
-      <c r="R2" t="n">
-        <v>1.787502084491367</v>
+      <c r="Q2" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="R2" s="1" t="n">
+        <v>1.778747513382372</v>
       </c>
       <c r="S2" t="n">
         <v>0</v>
@@ -605,18 +605,18 @@
         <v>0.5890486225480862</v>
       </c>
       <c r="V2" s="1" t="n">
-        <v>1.787502084491367</v>
+        <v>0.83675541816258</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.9181615599999999</v>
+        <v>0.9181615710258484</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.2147622</v>
-      </c>
-      <c r="C3" t="n">
-        <v>3.366405849427805</v>
+        <v>-0.2147622108459473</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D3" t="n">
         <v>8</v>
@@ -630,8 +630,8 @@
       <c r="G3" t="n">
         <v>0.8695652173913043</v>
       </c>
-      <c r="H3" t="n">
-        <v>15</v>
+      <c r="H3" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="I3" t="n">
         <v>0.1111111111111111</v>
@@ -642,8 +642,8 @@
       <c r="K3" t="n">
         <v>0.3882169059470468</v>
       </c>
-      <c r="L3" t="n">
-        <v>5</v>
+      <c r="L3" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="M3" t="n">
         <v>0.5</v>
@@ -657,8 +657,8 @@
       <c r="P3" t="n">
         <v>0.7027748523460556</v>
       </c>
-      <c r="Q3" t="n">
-        <v>5</v>
+      <c r="Q3" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="R3" t="n">
         <v>1.73023804570537</v>
@@ -673,18 +673,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V3" s="1" t="n">
-        <v>1.73023804570537</v>
+        <v>0.6661598584833751</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-0.2731795099999999</v>
+        <v>-0.2731795012950897</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.08585639499999989</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1.892028062899493</v>
+        <v>-0.08585639297962189</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="D4" t="n">
         <v>5</v>
@@ -698,8 +698,8 @@
       <c r="G4" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H4" t="n">
-        <v>3</v>
+      <c r="H4" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="I4" t="n">
         <v>0.03401360544217687</v>
@@ -725,11 +725,11 @@
       <c r="P4" t="n">
         <v>0.3105674139582154</v>
       </c>
-      <c r="Q4" t="n">
-        <v>5</v>
-      </c>
-      <c r="R4" t="n">
-        <v>1.73023804570537</v>
+      <c r="Q4" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="R4" s="1" t="n">
+        <v>1.836011552168369</v>
       </c>
       <c r="S4" t="n">
         <v>0</v>
@@ -741,18 +741,18 @@
         <v>0.5890486225480862</v>
       </c>
       <c r="V4" s="1" t="n">
-        <v>1.73023804570537</v>
+        <v>0.8650730109199346</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.04841110333333317</v>
+        <v>0.04841111103693644</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.45007978</v>
-      </c>
-      <c r="C5" t="n">
-        <v>3.563430865515642</v>
+        <v>-0.4500797390937805</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D5" t="n">
         <v>10</v>
@@ -766,8 +766,8 @@
       <c r="G5" t="n">
         <v>0.8695652173913043</v>
       </c>
-      <c r="H5" t="n">
-        <v>13</v>
+      <c r="H5" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="I5" t="n">
         <v>0.1111111111111111</v>
@@ -793,8 +793,8 @@
       <c r="P5" t="n">
         <v>0.804047159219282</v>
       </c>
-      <c r="Q5" t="n">
-        <v>6</v>
+      <c r="Q5" s="1" t="n">
+        <v>13</v>
       </c>
       <c r="R5" t="n">
         <v>1.605420035791506</v>
@@ -809,18 +809,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V5" s="1" t="n">
-        <v>1.605420035791506</v>
+        <v>0.64830914455489</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.4263789999999999</v>
+        <v>0.4263790249824524</v>
       </c>
       <c r="B6" t="n">
-        <v>0.5725660999999999</v>
-      </c>
-      <c r="C6" t="n">
-        <v>3.362548187845878</v>
+        <v>0.5725660920143127</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D6" t="n">
         <v>7</v>
@@ -834,8 +834,8 @@
       <c r="G6" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H6" t="n">
-        <v>16</v>
+      <c r="H6" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="I6" t="n">
         <v>0.1111111111111111</v>
@@ -846,8 +846,8 @@
       <c r="K6" t="n">
         <v>0.3184052155890569</v>
       </c>
-      <c r="L6" t="n">
-        <v>5</v>
+      <c r="L6" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="M6" t="n">
         <v>0.5</v>
@@ -861,8 +861,8 @@
       <c r="P6" t="n">
         <v>0.6754849824949913</v>
       </c>
-      <c r="Q6" t="n">
-        <v>6</v>
+      <c r="Q6" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="R6" t="n">
         <v>1.73023804570537</v>
@@ -877,18 +877,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V6" s="1" t="n">
-        <v>1.73023804570537</v>
+        <v>0.6579459846693219</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-0.7939940000000001</v>
+        <v>-0.7939940094947815</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.3925162333333334</v>
-      </c>
-      <c r="C7" t="n">
-        <v>2.382430964585834</v>
+        <v>-0.3925162255764008</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="D7" t="n">
         <v>6</v>
@@ -905,14 +905,14 @@
       <c r="H7" t="n">
         <v>5</v>
       </c>
-      <c r="I7" t="n">
-        <v>0.04000000000000001</v>
+      <c r="I7" s="1" t="n">
+        <v>0.06666666666666668</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
       </c>
-      <c r="K7" t="n">
-        <v>0.07700552595579639</v>
+      <c r="K7" s="1" t="n">
+        <v>0.1665001124995195</v>
       </c>
       <c r="L7" t="n">
         <v>3</v>
@@ -932,8 +932,8 @@
       <c r="Q7" t="n">
         <v>5</v>
       </c>
-      <c r="R7" t="n">
-        <v>1.778747513382372</v>
+      <c r="R7" s="1" t="n">
+        <v>1.836011552168369</v>
       </c>
       <c r="S7" t="n">
         <v>0</v>
@@ -945,18 +945,18 @@
         <v>0.5890486225480862</v>
       </c>
       <c r="V7" s="1" t="n">
-        <v>1.778747513382372</v>
+        <v>0.7987001306267925</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.03616139999999995</v>
+        <v>0.0361613929271698</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.14251847</v>
-      </c>
-      <c r="C8" t="n">
-        <v>2.554511821968367</v>
+        <v>-0.142518475651741</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="D8" t="n">
         <v>7</v>
@@ -970,11 +970,11 @@
       <c r="G8" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H8" t="n">
-        <v>8</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.08000000000000002</v>
+      <c r="H8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>0.02666666666666668</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
@@ -997,11 +997,11 @@
       <c r="P8" t="n">
         <v>0.5978962573702267</v>
       </c>
-      <c r="Q8" t="n">
-        <v>7</v>
-      </c>
-      <c r="R8" t="n">
-        <v>1.847775752366145</v>
+      <c r="Q8" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="R8" s="1" t="n">
+        <v>1.83902118125715</v>
       </c>
       <c r="S8" t="n">
         <v>0</v>
@@ -1013,21 +1013,21 @@
         <v>0.3926990816987241</v>
       </c>
       <c r="V8" s="1" t="n">
-        <v>1.847775752366145</v>
+        <v>0.8669421343245584</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.9248767200000004</v>
+        <v>0.9248766899108887</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.3359417399999998</v>
-      </c>
-      <c r="C9" t="n">
-        <v>3.60814758879192</v>
-      </c>
-      <c r="D9" t="n">
-        <v>14</v>
+        <v>-0.3359417021274567</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="E9" t="n">
         <v>0.5731491830329671</v>
@@ -1038,8 +1038,8 @@
       <c r="G9" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H9" t="n">
-        <v>15</v>
+      <c r="H9" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="I9" t="n">
         <v>0.1111111111111111</v>
@@ -1065,8 +1065,8 @@
       <c r="P9" t="n">
         <v>0.7373254361100833</v>
       </c>
-      <c r="Q9" t="n">
-        <v>5</v>
+      <c r="Q9" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="R9" t="n">
         <v>1.73023804570537</v>
@@ -1081,21 +1081,21 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V9" s="1" t="n">
-        <v>1.73023804570537</v>
+        <v>0.6138210068641288</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.8390223100000004</v>
+        <v>0.8390222787857056</v>
       </c>
       <c r="B10" t="n">
-        <v>0.7052313650000003</v>
-      </c>
-      <c r="C10" t="n">
-        <v>3.62914081736388</v>
-      </c>
-      <c r="D10" t="n">
-        <v>14</v>
+        <v>0.7052313685417175</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="E10" t="n">
         <v>0.6079137608318881</v>
@@ -1106,11 +1106,11 @@
       <c r="G10" t="n">
         <v>0.8260869565217391</v>
       </c>
-      <c r="H10" t="n">
-        <v>16</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.07407407407407407</v>
+      <c r="H10" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>0.1111111111111111</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
@@ -1133,8 +1133,8 @@
       <c r="P10" t="n">
         <v>0.7404830606197635</v>
       </c>
-      <c r="Q10" t="n">
-        <v>5</v>
+      <c r="Q10" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="R10" t="n">
         <v>1.73023804570537</v>
@@ -1149,18 +1149,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V10" s="1" t="n">
-        <v>1.73023804570537</v>
+        <v>0.6005775785608443</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.9951859900000001</v>
+        <v>0.9951859712600708</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.1334540500000001</v>
-      </c>
-      <c r="C11" t="n">
-        <v>3.612271843445458</v>
+        <v>-0.1334540843963623</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D11" t="n">
         <v>10</v>
@@ -1174,8 +1174,8 @@
       <c r="G11" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H11" t="n">
-        <v>13</v>
+      <c r="H11" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="I11" t="n">
         <v>0.1111111111111111</v>
@@ -1184,7 +1184,7 @@
         <v>6</v>
       </c>
       <c r="K11" t="n">
-        <v>0.2851842039569112</v>
+        <v>0.2851842039569111</v>
       </c>
       <c r="L11" t="n">
         <v>5</v>
@@ -1201,8 +1201,8 @@
       <c r="P11" t="n">
         <v>0.8302763920018271</v>
       </c>
-      <c r="Q11" t="n">
-        <v>4</v>
+      <c r="Q11" s="1" t="n">
+        <v>13</v>
       </c>
       <c r="R11" t="n">
         <v>1.483611654966423</v>
@@ -1217,18 +1217,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V11" s="1" t="n">
-        <v>1.483611654966423</v>
+        <v>0.6521309403572546</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.5673130599999998</v>
+        <v>0.5673130750656128</v>
       </c>
       <c r="B12" t="n">
-        <v>-0.3635061800000001</v>
-      </c>
-      <c r="C12" t="n">
-        <v>3.101515551079539</v>
+        <v>-0.3635061681270599</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D12" t="n">
         <v>8</v>
@@ -1242,8 +1242,8 @@
       <c r="G12" t="n">
         <v>0.8695652173913043</v>
       </c>
-      <c r="H12" t="n">
-        <v>11</v>
+      <c r="H12" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="I12" t="n">
         <v>0.1111111111111111</v>
@@ -1251,8 +1251,8 @@
       <c r="J12" t="n">
         <v>5</v>
       </c>
-      <c r="K12" t="n">
-        <v>0.1647420788184441</v>
+      <c r="K12" s="1" t="n">
+        <v>0.2544603298412751</v>
       </c>
       <c r="L12" t="n">
         <v>4</v>
@@ -1269,8 +1269,8 @@
       <c r="P12" t="n">
         <v>0.7186019519514407</v>
       </c>
-      <c r="Q12" t="n">
-        <v>4</v>
+      <c r="Q12" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="R12" t="n">
         <v>1.911059049329703</v>
@@ -1285,18 +1285,18 @@
         <v>0.3926990816987241</v>
       </c>
       <c r="V12" s="1" t="n">
-        <v>1.911059049329703</v>
+        <v>0.7370563993323642</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.9194077000000004</v>
+        <v>0.9194077253341675</v>
       </c>
       <c r="B13" t="n">
-        <v>-1.51476195</v>
-      </c>
-      <c r="C13" t="n">
-        <v>3.207435887865077</v>
+        <v>-1.514761924743652</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D13" t="n">
         <v>8</v>
@@ -1310,8 +1310,8 @@
       <c r="G13" t="n">
         <v>0.9565217391304348</v>
       </c>
-      <c r="H13" t="n">
-        <v>16</v>
+      <c r="H13" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="I13" t="n">
         <v>0.1111111111111111</v>
@@ -1337,11 +1337,11 @@
       <c r="P13" t="n">
         <v>0.6788710458531927</v>
       </c>
-      <c r="Q13" t="n">
-        <v>5</v>
+      <c r="Q13" s="1" t="n">
+        <v>17</v>
       </c>
       <c r="R13" t="n">
-        <v>1.790511713580147</v>
+        <v>1.790511713580148</v>
       </c>
       <c r="S13" t="n">
         <v>0</v>
@@ -1353,18 +1353,18 @@
         <v>0.3926990816987241</v>
       </c>
       <c r="V13" s="1" t="n">
-        <v>1.790511713580147</v>
+        <v>0.6983743624362077</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.4215589300000001</v>
+        <v>0.4215589165687561</v>
       </c>
       <c r="B14" t="n">
-        <v>0.568173275</v>
-      </c>
-      <c r="C14" t="n">
-        <v>3.360703915185088</v>
+        <v>0.5681732892990112</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D14" t="n">
         <v>8</v>
@@ -1378,8 +1378,8 @@
       <c r="G14" t="n">
         <v>0.8695652173913043</v>
       </c>
-      <c r="H14" t="n">
-        <v>15</v>
+      <c r="H14" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="I14" t="n">
         <v>0.1111111111111111</v>
@@ -1405,8 +1405,8 @@
       <c r="P14" t="n">
         <v>0.6784647622519333</v>
       </c>
-      <c r="Q14" t="n">
-        <v>6</v>
+      <c r="Q14" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="R14" t="n">
         <v>1.73023804570537</v>
@@ -1421,21 +1421,21 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V14" s="1" t="n">
-        <v>1.73023804570537</v>
+        <v>0.6650094846093758</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.9014067199999997</v>
+        <v>0.9014067053794861</v>
       </c>
       <c r="B15" t="n">
-        <v>0.6141835399999998</v>
-      </c>
-      <c r="C15" t="n">
-        <v>3.567474840785243</v>
-      </c>
-      <c r="D15" t="n">
-        <v>9</v>
+        <v>0.6141835153102875</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="E15" t="n">
         <v>0.5102222561629912</v>
@@ -1446,8 +1446,8 @@
       <c r="G15" t="n">
         <v>0.8260869565217391</v>
       </c>
-      <c r="H15" t="n">
-        <v>15</v>
+      <c r="H15" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="I15" t="n">
         <v>0.1111111111111111</v>
@@ -1458,8 +1458,8 @@
       <c r="K15" t="n">
         <v>0.2469973958198823</v>
       </c>
-      <c r="L15" t="n">
-        <v>5</v>
+      <c r="L15" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="M15" t="n">
         <v>0.5</v>
@@ -1473,8 +1473,8 @@
       <c r="P15" t="n">
         <v>0.7637942340039413</v>
       </c>
-      <c r="Q15" t="n">
-        <v>3</v>
+      <c r="Q15" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="R15" t="n">
         <v>1.665693703666284</v>
@@ -1489,18 +1489,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V15" s="1" t="n">
-        <v>1.665693703666284</v>
+        <v>0.641250713759876</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.48245478</v>
+        <v>0.482454776763916</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.43907484</v>
-      </c>
-      <c r="C16" t="n">
-        <v>3.327650915676295</v>
+        <v>-0.4390748143196106</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D16" t="n">
         <v>8</v>
@@ -1514,8 +1514,8 @@
       <c r="G16" t="n">
         <v>0.8695652173913043</v>
       </c>
-      <c r="H16" t="n">
-        <v>15</v>
+      <c r="H16" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="I16" t="n">
         <v>0.1111111111111111</v>
@@ -1526,8 +1526,8 @@
       <c r="K16" t="n">
         <v>0.4798044244031647</v>
       </c>
-      <c r="L16" t="n">
-        <v>5</v>
+      <c r="L16" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="M16" t="n">
         <v>0.5</v>
@@ -1541,11 +1541,11 @@
       <c r="P16" t="n">
         <v>0.6834612805791206</v>
       </c>
-      <c r="Q16" t="n">
-        <v>4</v>
-      </c>
-      <c r="R16" t="n">
-        <v>1.730238045705369</v>
+      <c r="Q16" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="R16" s="1" t="n">
+        <v>1.790511713580148</v>
       </c>
       <c r="S16" t="n">
         <v>0</v>
@@ -1557,18 +1557,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V16" s="1" t="n">
-        <v>1.730238045705369</v>
+        <v>0.6684719718814343</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>-0.6170376999999999</v>
+        <v>-0.6170377135276794</v>
       </c>
       <c r="B17" t="n">
-        <v>-0.4183956999999998</v>
-      </c>
-      <c r="C17" t="n">
-        <v>2.46380717380268</v>
+        <v>-0.4183956980705261</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="D17" t="n">
         <v>6</v>
@@ -1585,8 +1585,8 @@
       <c r="H17" t="n">
         <v>5</v>
       </c>
-      <c r="I17" t="n">
-        <v>0.04000000000000001</v>
+      <c r="I17" s="1" t="n">
+        <v>0.06666666666666668</v>
       </c>
       <c r="J17" t="n">
         <v>0</v>
@@ -1612,8 +1612,8 @@
       <c r="Q17" t="n">
         <v>5</v>
       </c>
-      <c r="R17" t="n">
-        <v>1.819976677806285</v>
+      <c r="R17" s="1" t="n">
+        <v>1.836011552168369</v>
       </c>
       <c r="S17" t="n">
         <v>0</v>
@@ -1625,18 +1625,18 @@
         <v>0.5890486225480862</v>
       </c>
       <c r="V17" s="1" t="n">
-        <v>1.819976677806285</v>
+        <v>0.7485155768993137</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>-0.08364505000000005</v>
+        <v>-0.0836450606584549</v>
       </c>
       <c r="B18" t="n">
-        <v>0.769534525</v>
-      </c>
-      <c r="C18" t="n">
-        <v>3.302967493968384</v>
+        <v>0.7695344835519791</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D18" t="n">
         <v>6</v>
@@ -1650,8 +1650,8 @@
       <c r="G18" t="n">
         <v>0.9565217391304348</v>
       </c>
-      <c r="H18" t="n">
-        <v>7</v>
+      <c r="H18" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="I18" t="n">
         <v>0.1111111111111111</v>
@@ -1662,8 +1662,8 @@
       <c r="K18" t="n">
         <v>0.1917169586584434</v>
       </c>
-      <c r="L18" t="n">
-        <v>4</v>
+      <c r="L18" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="M18" t="n">
         <v>0.5</v>
@@ -1677,8 +1677,8 @@
       <c r="P18" t="n">
         <v>0.6190143854148003</v>
       </c>
-      <c r="Q18" t="n">
-        <v>5</v>
+      <c r="Q18" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="R18" t="n">
         <v>1.778747513382372</v>
@@ -1693,18 +1693,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V18" s="1" t="n">
-        <v>1.778747513382372</v>
+        <v>0.7044351695646405</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>-0.5223600700000001</v>
+        <v>-0.52236008644104</v>
       </c>
       <c r="B19" t="n">
-        <v>-0.3625948150000001</v>
-      </c>
-      <c r="C19" t="n">
-        <v>3.29584809957333</v>
+        <v>-0.3625948131084442</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D19" t="n">
         <v>6</v>
@@ -1718,8 +1718,8 @@
       <c r="G19" t="n">
         <v>0.8260869565217391</v>
       </c>
-      <c r="H19" t="n">
-        <v>6</v>
+      <c r="H19" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="I19" t="n">
         <v>0.1666666666666667</v>
@@ -1730,8 +1730,8 @@
       <c r="K19" t="n">
         <v>0.3082695217564364</v>
       </c>
-      <c r="L19" t="n">
-        <v>4</v>
+      <c r="L19" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="M19" t="n">
         <v>0.3</v>
@@ -1745,8 +1745,8 @@
       <c r="P19" t="n">
         <v>0.6217645988052942</v>
       </c>
-      <c r="Q19" t="n">
-        <v>4</v>
+      <c r="Q19" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="R19" t="n">
         <v>1.714203171343286</v>
@@ -1761,21 +1761,21 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V19" s="1" t="n">
-        <v>1.714203171343286</v>
+        <v>0.6885317715154339</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.4413055900000004</v>
+        <v>0.4413056075572968</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.4143381199999997</v>
-      </c>
-      <c r="C20" t="n">
-        <v>3.607711490568475</v>
-      </c>
-      <c r="D20" t="n">
-        <v>9</v>
+        <v>-0.4143381118774414</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="E20" t="n">
         <v>0.6555682270823208</v>
@@ -1786,8 +1786,8 @@
       <c r="G20" t="n">
         <v>0.7826086956521739</v>
       </c>
-      <c r="H20" t="n">
-        <v>15</v>
+      <c r="H20" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="I20" t="n">
         <v>0.1111111111111111</v>
@@ -1798,8 +1798,8 @@
       <c r="K20" t="n">
         <v>0.4481460856785227</v>
       </c>
-      <c r="L20" t="n">
-        <v>5</v>
+      <c r="L20" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="M20" t="n">
         <v>0.5</v>
@@ -1813,8 +1813,8 @@
       <c r="P20" t="n">
         <v>0.8088382236805132</v>
       </c>
-      <c r="Q20" t="n">
-        <v>5</v>
+      <c r="Q20" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="R20" t="n">
         <v>1.483611654966423</v>
@@ -1829,21 +1829,21 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V20" s="1" t="n">
-        <v>1.483611654966423</v>
+        <v>0.6302777775694512</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.4340425700000002</v>
+        <v>0.4340425729751587</v>
       </c>
       <c r="B21" t="n">
-        <v>0.5762800250000002</v>
-      </c>
-      <c r="C21" t="n">
-        <v>3.536727884349005</v>
-      </c>
-      <c r="D21" t="n">
-        <v>14</v>
+        <v>0.5762799978256226</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="E21" t="n">
         <v>0.5339198095168153</v>
@@ -1854,11 +1854,11 @@
       <c r="G21" t="n">
         <v>0.7826086956521739</v>
       </c>
-      <c r="H21" t="n">
-        <v>15</v>
-      </c>
-      <c r="I21" t="n">
-        <v>0.07407407407407407</v>
+      <c r="H21" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I21" s="1" t="n">
+        <v>0.1111111111111111</v>
       </c>
       <c r="J21" t="n">
         <v>0</v>
@@ -1881,8 +1881,8 @@
       <c r="P21" t="n">
         <v>0.7202343528225197</v>
       </c>
-      <c r="Q21" t="n">
-        <v>6</v>
+      <c r="Q21" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="R21" t="n">
         <v>1.73023804570537</v>
@@ -1897,18 +1897,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V21" s="1" t="n">
-        <v>1.73023804570537</v>
+        <v>0.6335793307294701</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.8834339299999999</v>
+        <v>0.8834339380264282</v>
       </c>
       <c r="B22" t="n">
-        <v>1.023428165</v>
-      </c>
-      <c r="C22" t="n">
-        <v>3.390699711167795</v>
+        <v>1.023428201675415</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D22" t="n">
         <v>8</v>
@@ -1922,8 +1922,8 @@
       <c r="G22" t="n">
         <v>0.8260869565217391</v>
       </c>
-      <c r="H22" t="n">
-        <v>15</v>
+      <c r="H22" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="I22" t="n">
         <v>0.1111111111111111</v>
@@ -1932,7 +1932,7 @@
         <v>0</v>
       </c>
       <c r="K22" t="n">
-        <v>0.419577683632445</v>
+        <v>0.4195776836324451</v>
       </c>
       <c r="L22" t="n">
         <v>4</v>
@@ -1949,11 +1949,11 @@
       <c r="P22" t="n">
         <v>0.7093218955161197</v>
       </c>
-      <c r="Q22" t="n">
-        <v>5</v>
+      <c r="Q22" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="R22" t="n">
-        <v>1.790511713580147</v>
+        <v>1.790511713580148</v>
       </c>
       <c r="S22" t="n">
         <v>0</v>
@@ -1965,21 +1965,21 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V22" s="1" t="n">
-        <v>1.790511713580147</v>
+        <v>0.6511065600306005</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.4954316000000002</v>
+        <v>0.4954316020011902</v>
       </c>
       <c r="B23" t="n">
-        <v>0.6457960500000003</v>
-      </c>
-      <c r="C23" t="n">
-        <v>3.483901008448568</v>
-      </c>
-      <c r="D23" t="n">
-        <v>9</v>
+        <v>0.6457960605621338</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="E23" t="n">
         <v>0.5744675483392004</v>
@@ -1990,8 +1990,8 @@
       <c r="G23" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H23" t="n">
-        <v>15</v>
+      <c r="H23" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="I23" t="n">
         <v>0.1111111111111111</v>
@@ -2017,8 +2017,8 @@
       <c r="P23" t="n">
         <v>0.7978298655752953</v>
       </c>
-      <c r="Q23" t="n">
-        <v>6</v>
+      <c r="Q23" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="R23" t="n">
         <v>1.483611654966423</v>
@@ -2033,18 +2033,18 @@
         <v>0.3926990816987241</v>
       </c>
       <c r="V23" s="1" t="n">
-        <v>1.483611654966423</v>
+        <v>0.650165701616685</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.3267729199999999</v>
+        <v>0.326772928237915</v>
       </c>
       <c r="B24" t="n">
-        <v>0.4680099999999998</v>
-      </c>
-      <c r="C24" t="n">
-        <v>3.321347433155015</v>
+        <v>0.4680100083351135</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D24" t="n">
         <v>7</v>
@@ -2058,8 +2058,8 @@
       <c r="G24" t="n">
         <v>0.8695652173913043</v>
       </c>
-      <c r="H24" t="n">
-        <v>16</v>
+      <c r="H24" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="I24" t="n">
         <v>0.1111111111111111</v>
@@ -2085,11 +2085,11 @@
       <c r="P24" t="n">
         <v>0.6923145921415631</v>
       </c>
-      <c r="Q24" t="n">
-        <v>5</v>
+      <c r="Q24" s="1" t="n">
+        <v>17</v>
       </c>
       <c r="R24" t="n">
-        <v>1.790511713580147</v>
+        <v>1.790511713580148</v>
       </c>
       <c r="S24" t="n">
         <v>0</v>
@@ -2101,18 +2101,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V24" s="1" t="n">
-        <v>1.790511713580147</v>
+        <v>0.6634989640766628</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.5158521600000003</v>
+        <v>0.5158521570265293</v>
       </c>
       <c r="B25" t="n">
-        <v>-0.1740317966666664</v>
-      </c>
-      <c r="C25" t="n">
-        <v>3.298212236796929</v>
+        <v>-0.1740318139394124</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D25" t="n">
         <v>8</v>
@@ -2126,8 +2126,8 @@
       <c r="G25" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H25" t="n">
-        <v>15</v>
+      <c r="H25" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="I25" t="n">
         <v>0.1111111111111111</v>
@@ -2138,8 +2138,8 @@
       <c r="K25" t="n">
         <v>0.3525351912503066</v>
       </c>
-      <c r="L25" t="n">
-        <v>5</v>
+      <c r="L25" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="M25" t="n">
         <v>0.5</v>
@@ -2153,8 +2153,8 @@
       <c r="P25" t="n">
         <v>0.656506326906396</v>
       </c>
-      <c r="Q25" t="n">
-        <v>4</v>
+      <c r="Q25" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="R25" t="n">
         <v>1.605420035791506</v>
@@ -2169,18 +2169,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V25" s="1" t="n">
-        <v>1.605420035791506</v>
+        <v>0.6830557184245316</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.50498815</v>
+        <v>0.5049881339073181</v>
       </c>
       <c r="B26" t="n">
-        <v>0.3508234749999999</v>
-      </c>
-      <c r="C26" t="n">
-        <v>3.201355389290226</v>
+        <v>0.3508234620094299</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D26" t="n">
         <v>7</v>
@@ -2194,8 +2194,8 @@
       <c r="G26" t="n">
         <v>0.9565217391304348</v>
       </c>
-      <c r="H26" t="n">
-        <v>16</v>
+      <c r="H26" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="I26" t="n">
         <v>0.0625</v>
@@ -2221,8 +2221,8 @@
       <c r="P26" t="n">
         <v>0.6636836025590529</v>
       </c>
-      <c r="Q26" t="n">
-        <v>5</v>
+      <c r="Q26" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="R26" t="n">
         <v>1.73023804570537</v>
@@ -2237,18 +2237,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V26" s="1" t="n">
-        <v>1.73023804570537</v>
+        <v>0.6896461033058153</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>-0.52596591</v>
+        <v>-0.5259659290313721</v>
       </c>
       <c r="B27" t="n">
-        <v>-0.364647295</v>
-      </c>
-      <c r="C27" t="n">
-        <v>2.33780441506125</v>
+        <v>-0.3646472990512848</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="D27" t="n">
         <v>6</v>
@@ -2262,8 +2262,8 @@
       <c r="G27" t="n">
         <v>0.9565217391304348</v>
       </c>
-      <c r="H27" t="n">
-        <v>7</v>
+      <c r="H27" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="I27" t="n">
         <v>0.04000000000000001</v>
@@ -2289,8 +2289,8 @@
       <c r="P27" t="n">
         <v>0.4337770710588943</v>
       </c>
-      <c r="Q27" t="n">
-        <v>5</v>
+      <c r="Q27" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="R27" t="n">
         <v>1.83902118125715</v>
@@ -2305,18 +2305,18 @@
         <v>0.5890486225480862</v>
       </c>
       <c r="V27" s="1" t="n">
-        <v>1.83902118125715</v>
+        <v>0.9075594004019465</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.4819525899999998</v>
+        <v>0.481952577829361</v>
       </c>
       <c r="B28" t="n">
-        <v>0.3304328549999998</v>
-      </c>
-      <c r="C28" t="n">
-        <v>3.233981299862188</v>
+        <v>0.3304328322410583</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D28" t="n">
         <v>7</v>
@@ -2330,8 +2330,8 @@
       <c r="G28" t="n">
         <v>0.8260869565217391</v>
       </c>
-      <c r="H28" t="n">
-        <v>15</v>
+      <c r="H28" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="I28" t="n">
         <v>0.1111111111111111</v>
@@ -2357,8 +2357,8 @@
       <c r="P28" t="n">
         <v>0.6743069499229292</v>
       </c>
-      <c r="Q28" t="n">
-        <v>4</v>
+      <c r="Q28" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="R28" t="n">
         <v>1.73023804570537</v>
@@ -2373,18 +2373,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V28" s="1" t="n">
-        <v>1.73023804570537</v>
+        <v>0.6843983003032706</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1.05846318</v>
+        <v>1.058463215827942</v>
       </c>
       <c r="B29" t="n">
-        <v>1.20907454</v>
-      </c>
-      <c r="C29" t="n">
-        <v>3.568041929897631</v>
+        <v>1.2090744972229</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D29" t="n">
         <v>9</v>
@@ -2398,8 +2398,8 @@
       <c r="G29" t="n">
         <v>0.9565217391304348</v>
       </c>
-      <c r="H29" t="n">
-        <v>12</v>
+      <c r="H29" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="I29" t="n">
         <v>0.1111111111111111</v>
@@ -2425,8 +2425,8 @@
       <c r="P29" t="n">
         <v>0.8349861566943183</v>
       </c>
-      <c r="Q29" t="n">
-        <v>5</v>
+      <c r="Q29" s="1" t="n">
+        <v>12</v>
       </c>
       <c r="R29" t="n">
         <v>1.714203171343286</v>
@@ -2441,21 +2441,21 @@
         <v>0.3926990816987241</v>
       </c>
       <c r="V29" s="1" t="n">
-        <v>1.714203171343286</v>
+        <v>0.6592202618662243</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.4745493600000001</v>
+        <v>0.4745493531227112</v>
       </c>
       <c r="B30" t="n">
-        <v>0.32328257</v>
-      </c>
-      <c r="C30" t="n">
-        <v>3.500883110436085</v>
-      </c>
-      <c r="D30" t="n">
-        <v>9</v>
+        <v>0.3232825696468353</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="E30" t="n">
         <v>0.6382947949961563</v>
@@ -2466,8 +2466,8 @@
       <c r="G30" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H30" t="n">
-        <v>15</v>
+      <c r="H30" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="I30" t="n">
         <v>0.1111111111111111</v>
@@ -2493,8 +2493,8 @@
       <c r="P30" t="n">
         <v>0.7789099676396366</v>
       </c>
-      <c r="Q30" t="n">
-        <v>5</v>
+      <c r="Q30" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="R30" t="n">
         <v>1.605420035791506</v>
@@ -2509,18 +2509,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V30" s="1" t="n">
-        <v>1.605420035791506</v>
+        <v>0.6357230137414817</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.5321021099999999</v>
+        <v>0.532102108001709</v>
       </c>
       <c r="B31" t="n">
-        <v>0.3791253449999999</v>
-      </c>
-      <c r="C31" t="n">
-        <v>3.338404170413899</v>
+        <v>0.3791253566741943</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D31" t="n">
         <v>8</v>
@@ -2534,8 +2534,8 @@
       <c r="G31" t="n">
         <v>0.8260869565217391</v>
       </c>
-      <c r="H31" t="n">
-        <v>15</v>
+      <c r="H31" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="I31" t="n">
         <v>0.1111111111111111</v>
@@ -2546,8 +2546,8 @@
       <c r="K31" t="n">
         <v>0.3250411085106832</v>
       </c>
-      <c r="L31" t="n">
-        <v>5</v>
+      <c r="L31" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="M31" t="n">
         <v>0.5</v>
@@ -2561,8 +2561,8 @@
       <c r="P31" t="n">
         <v>0.6814860262368827</v>
       </c>
-      <c r="Q31" t="n">
-        <v>4</v>
+      <c r="Q31" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="R31" t="n">
         <v>1.665693703666284</v>
@@ -2577,18 +2577,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V31" s="1" t="n">
-        <v>1.665693703666284</v>
+        <v>0.6692841971169188</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.8871373599999999</v>
+        <v>0.8871374130249023</v>
       </c>
       <c r="B32" t="n">
-        <v>1.02721168</v>
-      </c>
-      <c r="C32" t="n">
-        <v>3.472896335947613</v>
+        <v>1.027211666107178</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D32" t="n">
         <v>8</v>
@@ -2602,8 +2602,8 @@
       <c r="G32" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H32" t="n">
-        <v>15</v>
+      <c r="H32" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="I32" t="n">
         <v>0.1111111111111111</v>
@@ -2614,8 +2614,8 @@
       <c r="K32" t="n">
         <v>0.2697406285597465</v>
       </c>
-      <c r="L32" t="n">
-        <v>5</v>
+      <c r="L32" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="M32" t="n">
         <v>0.6666666666666666</v>
@@ -2629,8 +2629,8 @@
       <c r="P32" t="n">
         <v>0.7112305104666558</v>
       </c>
-      <c r="Q32" t="n">
-        <v>5</v>
+      <c r="Q32" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="R32" t="n">
         <v>1.73023804570537</v>
@@ -2645,18 +2645,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V32" s="1" t="n">
-        <v>1.73023804570537</v>
+        <v>0.6403723036187963</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>-0.75191867</v>
+        <v>-0.7519186735153198</v>
       </c>
       <c r="B33" t="n">
-        <v>-0.75191867</v>
-      </c>
-      <c r="C33" t="n">
-        <v>2.343855110735963</v>
+        <v>-0.7519186735153198</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="D33" t="n">
         <v>5</v>
@@ -2670,17 +2670,17 @@
       <c r="G33" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H33" t="n">
-        <v>5</v>
-      </c>
-      <c r="I33" t="n">
-        <v>0.04000000000000001</v>
+      <c r="H33" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I33" s="1" t="n">
+        <v>0.06666666666666668</v>
       </c>
       <c r="J33" t="n">
         <v>0</v>
       </c>
-      <c r="K33" t="n">
-        <v>0.1015929646639226</v>
+      <c r="K33" s="1" t="n">
+        <v>0.1464848369504443</v>
       </c>
       <c r="L33" t="n">
         <v>3</v>
@@ -2697,8 +2697,8 @@
       <c r="P33" t="n">
         <v>0.39634075014939</v>
       </c>
-      <c r="Q33" t="n">
-        <v>6</v>
+      <c r="Q33" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="R33" t="n">
         <v>1.885299500946812</v>
@@ -2713,18 +2713,18 @@
         <v>0.5890486225480862</v>
       </c>
       <c r="V33" s="1" t="n">
-        <v>1.885299500946812</v>
+        <v>0.8174712223479225</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1.02654829</v>
+        <v>1.026548266410828</v>
       </c>
       <c r="B34" t="n">
-        <v>-1.377173595</v>
-      </c>
-      <c r="C34" t="n">
-        <v>3.615486725843786</v>
+        <v>-1.377173662185669</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D34" t="n">
         <v>10</v>
@@ -2738,8 +2738,8 @@
       <c r="G34" t="n">
         <v>0.8260869565217391</v>
       </c>
-      <c r="H34" t="n">
-        <v>13</v>
+      <c r="H34" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="I34" t="n">
         <v>0.1111111111111111</v>
@@ -2765,8 +2765,8 @@
       <c r="P34" t="n">
         <v>0.8486668508358579</v>
       </c>
-      <c r="Q34" t="n">
-        <v>6</v>
+      <c r="Q34" s="1" t="n">
+        <v>13</v>
       </c>
       <c r="R34" t="n">
         <v>1.483611654966423</v>
@@ -2781,18 +2781,18 @@
         <v>0.3926990816987241</v>
       </c>
       <c r="V34" s="1" t="n">
-        <v>1.483611654966423</v>
+        <v>0.635935610366822</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>-0.5593282299999999</v>
+        <v>-0.5593281984329224</v>
       </c>
       <c r="B35" t="n">
-        <v>-0.8767848199999999</v>
-      </c>
-      <c r="C35" t="n">
-        <v>3.129042806420076</v>
+        <v>-0.8767848014831543</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D35" t="n">
         <v>6</v>
@@ -2806,8 +2806,8 @@
       <c r="G35" t="n">
         <v>0.9565217391304348</v>
       </c>
-      <c r="H35" t="n">
-        <v>6</v>
+      <c r="H35" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="I35" t="n">
         <v>0.1111111111111111</v>
@@ -2818,8 +2818,8 @@
       <c r="K35" t="n">
         <v>0.3782650100817441</v>
       </c>
-      <c r="L35" t="n">
-        <v>4</v>
+      <c r="L35" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="M35" t="n">
         <v>0.5</v>
@@ -2833,8 +2833,8 @@
       <c r="P35" t="n">
         <v>0.6054045887584985</v>
       </c>
-      <c r="Q35" t="n">
-        <v>4</v>
+      <c r="Q35" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="R35" t="n">
         <v>1.714203171343286</v>
@@ -2849,18 +2849,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V35" s="1" t="n">
-        <v>1.714203171343286</v>
+        <v>0.7222017470467508</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>-0.06989885000000007</v>
+        <v>-0.06989885866641998</v>
       </c>
       <c r="B36" t="n">
-        <v>0.1222102649999999</v>
-      </c>
-      <c r="C36" t="n">
-        <v>2.537765719726716</v>
+        <v>0.1222102642059326</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="D36" t="n">
         <v>6</v>
@@ -2874,17 +2874,17 @@
       <c r="G36" t="n">
         <v>0.9565217391304348</v>
       </c>
-      <c r="H36" t="n">
-        <v>7</v>
-      </c>
-      <c r="I36" t="n">
-        <v>0.08000000000000002</v>
+      <c r="H36" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I36" s="1" t="n">
+        <v>0.04000000000000001</v>
       </c>
       <c r="J36" t="n">
         <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>0.2157362186069349</v>
+        <v>0.215736218606935</v>
       </c>
       <c r="L36" t="n">
         <v>3</v>
@@ -2901,11 +2901,11 @@
       <c r="P36" t="n">
         <v>0.5705471799181075</v>
       </c>
-      <c r="Q36" t="n">
-        <v>5</v>
-      </c>
-      <c r="R36" t="n">
-        <v>1.994082636498592</v>
+      <c r="Q36" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="R36" s="1" t="n">
+        <v>1.813261632874258</v>
       </c>
       <c r="S36" t="n">
         <v>0</v>
@@ -2917,18 +2917,18 @@
         <v>0.3926990816987241</v>
       </c>
       <c r="V36" s="1" t="n">
-        <v>1.994082636498592</v>
+        <v>0.8744251823984155</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.9476113799999998</v>
+        <v>0.9476113319396973</v>
       </c>
       <c r="B37" t="n">
-        <v>-1.35373064</v>
-      </c>
-      <c r="C37" t="n">
-        <v>3.665129854005043</v>
+        <v>-1.35373067855835</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D37" t="n">
         <v>10</v>
@@ -2942,8 +2942,8 @@
       <c r="G37" t="n">
         <v>0.7826086956521739</v>
       </c>
-      <c r="H37" t="n">
-        <v>15</v>
+      <c r="H37" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="I37" t="n">
         <v>0.1111111111111111</v>
@@ -2952,7 +2952,7 @@
         <v>6</v>
       </c>
       <c r="K37" t="n">
-        <v>0.3719056428795899</v>
+        <v>0.37190564287959</v>
       </c>
       <c r="L37" t="n">
         <v>5</v>
@@ -2969,8 +2969,8 @@
       <c r="P37" t="n">
         <v>0.8204341074181251</v>
       </c>
-      <c r="Q37" t="n">
-        <v>6</v>
+      <c r="Q37" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="R37" t="n">
         <v>1.605420035791506</v>
@@ -2985,21 +2985,21 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V37" s="1" t="n">
-        <v>1.605420035791506</v>
+        <v>0.6291603062906093</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.8294642799999999</v>
+        <v>0.829464316368103</v>
       </c>
       <c r="B38" t="n">
-        <v>0.06383097333333336</v>
-      </c>
-      <c r="C38" t="n">
-        <v>3.798567680915832</v>
-      </c>
-      <c r="D38" t="n">
-        <v>14</v>
+        <v>0.06383097171783447</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="E38" t="n">
         <v>0.6723319593699535</v>
@@ -3010,11 +3010,11 @@
       <c r="G38" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H38" t="n">
-        <v>15</v>
-      </c>
-      <c r="I38" t="n">
-        <v>0.07407407407407407</v>
+      <c r="H38" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="I38" s="1" t="n">
+        <v>0.1111111111111111</v>
       </c>
       <c r="J38" t="n">
         <v>0</v>
@@ -3037,11 +3037,11 @@
       <c r="P38" t="n">
         <v>0.7641136498668536</v>
       </c>
-      <c r="Q38" t="n">
-        <v>4</v>
+      <c r="Q38" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="R38" t="n">
-        <v>1.790511713580147</v>
+        <v>1.790511713580148</v>
       </c>
       <c r="S38" t="n">
         <v>0</v>
@@ -3053,18 +3053,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V38" s="1" t="n">
-        <v>1.790511713580147</v>
+        <v>0.5868051223459461</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.2081013499999999</v>
+        <v>0.2081013470888138</v>
       </c>
       <c r="B39" t="n">
-        <v>0.005945734999999924</v>
-      </c>
-      <c r="C39" t="n">
-        <v>2.304699202822833</v>
+        <v>0.005945734679698944</v>
+      </c>
+      <c r="C39" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="D39" t="n">
         <v>6</v>
@@ -3078,11 +3078,11 @@
       <c r="G39" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H39" t="n">
-        <v>7</v>
-      </c>
-      <c r="I39" t="n">
-        <v>0.08000000000000002</v>
+      <c r="H39" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I39" s="1" t="n">
+        <v>0.02666666666666668</v>
       </c>
       <c r="J39" t="n">
         <v>0</v>
@@ -3105,8 +3105,8 @@
       <c r="P39" t="n">
         <v>0.5202304725836779</v>
       </c>
-      <c r="Q39" t="n">
-        <v>5</v>
+      <c r="Q39" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="R39" t="n">
         <v>1.73023804570537</v>
@@ -3121,18 +3121,18 @@
         <v>0.3926990816987241</v>
       </c>
       <c r="V39" s="1" t="n">
-        <v>1.73023804570537</v>
+        <v>0.9329675001352364</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.4456265499999999</v>
+        <v>0.4456265568733215</v>
       </c>
       <c r="B40" t="n">
-        <v>0.5940335749999999</v>
-      </c>
-      <c r="C40" t="n">
-        <v>3.454050303961275</v>
+        <v>0.5940335988998413</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D40" t="n">
         <v>8</v>
@@ -3146,11 +3146,11 @@
       <c r="G40" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H40" t="n">
-        <v>15</v>
-      </c>
-      <c r="I40" t="n">
-        <v>0.07407407407407407</v>
+      <c r="H40" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I40" s="1" t="n">
+        <v>0.1111111111111111</v>
       </c>
       <c r="J40" t="n">
         <v>0</v>
@@ -3173,8 +3173,8 @@
       <c r="P40" t="n">
         <v>0.6995154028463711</v>
       </c>
-      <c r="Q40" t="n">
-        <v>6</v>
+      <c r="Q40" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="R40" t="n">
         <v>1.665693703666284</v>
@@ -3189,21 +3189,21 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V40" s="1" t="n">
-        <v>1.665693703666284</v>
+        <v>0.6480806958215264</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0.9586377399999997</v>
+        <v>0.9586377143859863</v>
       </c>
       <c r="B41" t="n">
-        <v>0.2458418399999998</v>
-      </c>
-      <c r="C41" t="n">
-        <v>3.875854816256313</v>
-      </c>
-      <c r="D41" t="n">
-        <v>10</v>
+        <v>0.2458418309688568</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <v>12</v>
       </c>
       <c r="E41" t="n">
         <v>0.6112831059678279</v>
@@ -3214,8 +3214,8 @@
       <c r="G41" t="n">
         <v>0.9565217391304348</v>
       </c>
-      <c r="H41" t="n">
-        <v>15</v>
+      <c r="H41" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="I41" t="n">
         <v>0.1111111111111111</v>
@@ -3241,8 +3241,8 @@
       <c r="P41" t="n">
         <v>0.8315490457628903</v>
       </c>
-      <c r="Q41" t="n">
-        <v>5</v>
+      <c r="Q41" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="R41" t="n">
         <v>1.605420035791506</v>
@@ -3257,18 +3257,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V41" s="1" t="n">
-        <v>1.605420035791506</v>
+        <v>0.5901100887283176</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>-0.3807920300000001</v>
+        <v>-0.3807920217514038</v>
       </c>
       <c r="B42" t="n">
-        <v>-0.553349775</v>
-      </c>
-      <c r="C42" t="n">
-        <v>2.696669311724185</v>
+        <v>-0.5533497830231985</v>
+      </c>
+      <c r="C42" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="D42" t="n">
         <v>5</v>
@@ -3282,8 +3282,8 @@
       <c r="G42" t="n">
         <v>1</v>
       </c>
-      <c r="H42" t="n">
-        <v>6</v>
+      <c r="H42" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="I42" t="n">
         <v>0.1041666666666667</v>
@@ -3294,8 +3294,8 @@
       <c r="K42" t="n">
         <v>0.1710310314731136</v>
       </c>
-      <c r="L42" t="n">
-        <v>4</v>
+      <c r="L42" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="M42" t="n">
         <v>0.4</v>
@@ -3309,8 +3309,8 @@
       <c r="P42" t="n">
         <v>0.4987382332235186</v>
       </c>
-      <c r="Q42" t="n">
-        <v>5</v>
+      <c r="Q42" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="R42" t="n">
         <v>1.714203171343286</v>
@@ -3325,18 +3325,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V42" s="1" t="n">
-        <v>1.714203171343286</v>
+        <v>0.8273935895550478</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>0.93603309</v>
+        <v>0.9360331296920776</v>
       </c>
       <c r="B43" t="n">
-        <v>-0.20132415</v>
-      </c>
-      <c r="C43" t="n">
-        <v>3.17485058778983</v>
+        <v>-0.2013241052627563</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D43" t="n">
         <v>7</v>
@@ -3350,8 +3350,8 @@
       <c r="G43" t="n">
         <v>0.8260869565217391</v>
       </c>
-      <c r="H43" t="n">
-        <v>15</v>
+      <c r="H43" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="I43" t="n">
         <v>0.0625</v>
@@ -3360,7 +3360,7 @@
         <v>0</v>
       </c>
       <c r="K43" t="n">
-        <v>0.3522948319246225</v>
+        <v>0.3522948319246226</v>
       </c>
       <c r="L43" t="n">
         <v>4</v>
@@ -3377,8 +3377,8 @@
       <c r="P43" t="n">
         <v>0.6574177797632969</v>
       </c>
-      <c r="Q43" t="n">
-        <v>5</v>
+      <c r="Q43" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="R43" t="n">
         <v>1.73023804570537</v>
@@ -3393,18 +3393,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V43" s="1" t="n">
-        <v>1.73023804570537</v>
+        <v>0.6902736568580091</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1.03380864</v>
+        <v>1.033808588981628</v>
       </c>
       <c r="B44" t="n">
-        <v>-1.38688732</v>
-      </c>
-      <c r="C44" t="n">
-        <v>3.784278734060136</v>
+        <v>-1.386887311935425</v>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D44" t="n">
         <v>9</v>
@@ -3418,8 +3418,8 @@
       <c r="G44" t="n">
         <v>0.9565217391304348</v>
       </c>
-      <c r="H44" t="n">
-        <v>15</v>
+      <c r="H44" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="I44" t="n">
         <v>0.1111111111111111</v>
@@ -3445,8 +3445,8 @@
       <c r="P44" t="n">
         <v>0.8321812764474428</v>
       </c>
-      <c r="Q44" t="n">
-        <v>5</v>
+      <c r="Q44" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="R44" t="n">
         <v>1.483611654966423</v>
@@ -3461,18 +3461,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V44" s="1" t="n">
-        <v>1.483611654966423</v>
+        <v>0.605031158695595</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>-0.05005424999999991</v>
+        <v>-0.05005425214767456</v>
       </c>
       <c r="B45" t="n">
-        <v>0.1232104350000001</v>
-      </c>
-      <c r="C45" t="n">
-        <v>2.516220442018226</v>
+        <v>0.1232104301452637</v>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="D45" t="n">
         <v>7</v>
@@ -3486,17 +3486,17 @@
       <c r="G45" t="n">
         <v>1</v>
       </c>
-      <c r="H45" t="n">
-        <v>9</v>
-      </c>
-      <c r="I45" t="n">
-        <v>0.04000000000000001</v>
+      <c r="H45" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I45" s="1" t="n">
+        <v>0.08000000000000002</v>
       </c>
       <c r="J45" t="n">
         <v>0</v>
       </c>
       <c r="K45" t="n">
-        <v>0.1107062314902389</v>
+        <v>0.1107062314902388</v>
       </c>
       <c r="L45" t="n">
         <v>3</v>
@@ -3513,11 +3513,11 @@
       <c r="P45" t="n">
         <v>0.543849356713797</v>
       </c>
-      <c r="Q45" t="n">
-        <v>5</v>
-      </c>
-      <c r="R45" t="n">
-        <v>1.834750507092842</v>
+      <c r="Q45" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="R45" s="1" t="n">
+        <v>1.548155997005509</v>
       </c>
       <c r="S45" t="n">
         <v>0</v>
@@ -3529,18 +3529,18 @@
         <v>0.3926990816987241</v>
       </c>
       <c r="V45" s="1" t="n">
-        <v>1.834750507092842</v>
+        <v>0.8506350837309871</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>0.4830367699999999</v>
+        <v>0.4830367565155029</v>
       </c>
       <c r="B46" t="n">
-        <v>-0.41171596</v>
-      </c>
-      <c r="C46" t="n">
-        <v>3.328159963226137</v>
+        <v>-0.4117159843444824</v>
+      </c>
+      <c r="C46" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D46" t="n">
         <v>8</v>
@@ -3554,11 +3554,11 @@
       <c r="G46" t="n">
         <v>0.8260869565217391</v>
       </c>
-      <c r="H46" t="n">
-        <v>15</v>
-      </c>
-      <c r="I46" t="n">
-        <v>0.07407407407407407</v>
+      <c r="H46" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="I46" s="1" t="n">
+        <v>0.1111111111111111</v>
       </c>
       <c r="J46" t="n">
         <v>0</v>
@@ -3566,8 +3566,8 @@
       <c r="K46" t="n">
         <v>0.545893415962606</v>
       </c>
-      <c r="L46" t="n">
-        <v>5</v>
+      <c r="L46" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="M46" t="n">
         <v>0.6666666666666666</v>
@@ -3581,11 +3581,11 @@
       <c r="P46" t="n">
         <v>0.662297742741271</v>
       </c>
-      <c r="Q46" t="n">
-        <v>4</v>
+      <c r="Q46" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="R46" t="n">
-        <v>1.730238045705369</v>
+        <v>1.73023804570537</v>
       </c>
       <c r="S46" t="n">
         <v>0</v>
@@ -3597,18 +3597,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V46" s="1" t="n">
-        <v>1.730238045705369</v>
+        <v>0.6662679161478898</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>-0.21169248</v>
+        <v>-0.2116924822330475</v>
       </c>
       <c r="B47" t="n">
-        <v>-1.34375754</v>
-      </c>
-      <c r="C47" t="n">
-        <v>3.515867256634603</v>
+        <v>-1.343757629394531</v>
+      </c>
+      <c r="C47" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D47" t="n">
         <v>9</v>
@@ -3622,8 +3622,8 @@
       <c r="G47" t="n">
         <v>0.8695652173913043</v>
       </c>
-      <c r="H47" t="n">
-        <v>13</v>
+      <c r="H47" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="I47" t="n">
         <v>0.1111111111111111</v>
@@ -3649,8 +3649,8 @@
       <c r="P47" t="n">
         <v>0.8179327885082108</v>
       </c>
-      <c r="Q47" t="n">
-        <v>5</v>
+      <c r="Q47" s="1" t="n">
+        <v>13</v>
       </c>
       <c r="R47" t="n">
         <v>1.483611654966423</v>
@@ -3665,18 +3665,18 @@
         <v>0.3926990816987241</v>
       </c>
       <c r="V47" s="1" t="n">
-        <v>1.483611654966423</v>
+        <v>0.6543345173352624</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>-0.36386627</v>
+        <v>-0.3638662695884705</v>
       </c>
       <c r="B48" t="n">
-        <v>-0.549917725</v>
-      </c>
-      <c r="C48" t="n">
-        <v>2.308693834093694</v>
+        <v>-0.5499176979064941</v>
+      </c>
+      <c r="C48" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="D48" t="n">
         <v>5</v>
@@ -3693,14 +3693,14 @@
       <c r="H48" t="n">
         <v>5</v>
       </c>
-      <c r="I48" t="n">
-        <v>0.04000000000000001</v>
+      <c r="I48" s="1" t="n">
+        <v>0.06666666666666668</v>
       </c>
       <c r="J48" t="n">
         <v>0</v>
       </c>
-      <c r="K48" t="n">
-        <v>0.1459203711394632</v>
+      <c r="K48" s="1" t="n">
+        <v>0.108581463814451</v>
       </c>
       <c r="L48" t="n">
         <v>3</v>
@@ -3733,21 +3733,21 @@
         <v>0.5890486225480862</v>
       </c>
       <c r="V48" s="1" t="n">
-        <v>1.836011552168369</v>
+        <v>0.8271754651982959</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1.00349232</v>
+        <v>1.00349235534668</v>
       </c>
       <c r="B49" t="n">
-        <v>-0.3411080399999999</v>
-      </c>
-      <c r="C49" t="n">
-        <v>3.60910994788932</v>
-      </c>
-      <c r="D49" t="n">
-        <v>9</v>
+        <v>-0.3411079943180084</v>
+      </c>
+      <c r="C49" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D49" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="E49" t="n">
         <v>0.624677493119521</v>
@@ -3758,8 +3758,8 @@
       <c r="G49" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H49" t="n">
-        <v>15</v>
+      <c r="H49" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="I49" t="n">
         <v>0.1111111111111111</v>
@@ -3768,7 +3768,7 @@
         <v>0</v>
       </c>
       <c r="K49" t="n">
-        <v>0.3762245716819117</v>
+        <v>0.3762245716819116</v>
       </c>
       <c r="L49" t="n">
         <v>4</v>
@@ -3785,8 +3785,8 @@
       <c r="P49" t="n">
         <v>0.8115764439333524</v>
       </c>
-      <c r="Q49" t="n">
-        <v>6</v>
+      <c r="Q49" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="R49" t="n">
         <v>1.483611654966423</v>
@@ -3801,18 +3801,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V49" s="1" t="n">
-        <v>1.483611654966423</v>
+        <v>0.6275847342922503</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>-0.81724544</v>
+        <v>-0.8172454237937927</v>
       </c>
       <c r="B50" t="n">
-        <v>-0.226774895</v>
-      </c>
-      <c r="C50" t="n">
-        <v>2.511637445451075</v>
+        <v>-0.2267749011516571</v>
+      </c>
+      <c r="C50" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="D50" t="n">
         <v>7</v>
@@ -3826,8 +3826,8 @@
       <c r="G50" t="n">
         <v>0.8695652173913043</v>
       </c>
-      <c r="H50" t="n">
-        <v>5</v>
+      <c r="H50" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="I50" t="n">
         <v>0.1041666666666667</v>
@@ -3853,11 +3853,11 @@
       <c r="P50" t="n">
         <v>0.4418276414378308</v>
       </c>
-      <c r="Q50" t="n">
-        <v>4</v>
-      </c>
-      <c r="R50" t="n">
-        <v>1.751726919923953</v>
+      <c r="Q50" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="R50" s="1" t="n">
+        <v>1.665693703666284</v>
       </c>
       <c r="S50" t="n">
         <v>0</v>
@@ -3869,18 +3869,18 @@
         <v>0.5890486225480862</v>
       </c>
       <c r="V50" s="1" t="n">
-        <v>1.751726919923953</v>
+        <v>0.7794775098306321</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>-0.5234944500000001</v>
+        <v>-0.5234944224357605</v>
       </c>
       <c r="B51" t="n">
-        <v>-0.363320775</v>
-      </c>
-      <c r="C51" t="n">
-        <v>2.333789217485165</v>
+        <v>-0.3633207678794861</v>
+      </c>
+      <c r="C51" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="D51" t="n">
         <v>6</v>
@@ -3894,11 +3894,11 @@
       <c r="G51" t="n">
         <v>0.8260869565217391</v>
       </c>
-      <c r="H51" t="n">
-        <v>7</v>
-      </c>
-      <c r="I51" t="n">
-        <v>0.08000000000000002</v>
+      <c r="H51" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I51" s="1" t="n">
+        <v>0.04000000000000001</v>
       </c>
       <c r="J51" t="n">
         <v>0</v>
@@ -3906,8 +3906,8 @@
       <c r="K51" t="n">
         <v>0.227749606934105</v>
       </c>
-      <c r="L51" t="n">
-        <v>3</v>
+      <c r="L51" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="M51" t="n">
         <v>0.75</v>
@@ -3921,8 +3921,8 @@
       <c r="P51" t="n">
         <v>0.4280771712004225</v>
       </c>
-      <c r="Q51" t="n">
-        <v>5</v>
+      <c r="Q51" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="R51" t="n">
         <v>1.548155997005509</v>
@@ -3937,18 +3937,18 @@
         <v>0.5890486225480862</v>
       </c>
       <c r="V51" s="1" t="n">
-        <v>1.548155997005509</v>
+        <v>0.9128642833246349</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>0.4997361399999998</v>
+        <v>0.4997361302375793</v>
       </c>
       <c r="B52" t="n">
-        <v>0.6527048499999998</v>
-      </c>
-      <c r="C52" t="n">
-        <v>3.34841032208782</v>
+        <v>0.6527048349380493</v>
+      </c>
+      <c r="C52" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D52" t="n">
         <v>8</v>
@@ -3962,11 +3962,11 @@
       <c r="G52" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H52" t="n">
-        <v>15</v>
-      </c>
-      <c r="I52" t="n">
-        <v>0.07407407407407407</v>
+      <c r="H52" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I52" s="1" t="n">
+        <v>0.1111111111111111</v>
       </c>
       <c r="J52" t="n">
         <v>0</v>
@@ -3989,8 +3989,8 @@
       <c r="P52" t="n">
         <v>0.6796055464304638</v>
       </c>
-      <c r="Q52" t="n">
-        <v>5</v>
+      <c r="Q52" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="R52" t="n">
         <v>1.548155997005509</v>
@@ -4005,18 +4005,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V52" s="1" t="n">
-        <v>1.548155997005509</v>
+        <v>0.6672121894559961</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>0.08208310000000008</v>
+        <v>0.08208309859037399</v>
       </c>
       <c r="B53" t="n">
-        <v>-0.08114496999999993</v>
-      </c>
-      <c r="C53" t="n">
-        <v>2.702405952858771</v>
+        <v>-0.08114497363567352</v>
+      </c>
+      <c r="C53" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="D53" t="n">
         <v>7</v>
@@ -4030,17 +4030,17 @@
       <c r="G53" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H53" t="n">
-        <v>7</v>
-      </c>
-      <c r="I53" t="n">
-        <v>0.1041666666666667</v>
+      <c r="H53" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I53" s="1" t="n">
+        <v>0.0625</v>
       </c>
       <c r="J53" t="n">
         <v>0</v>
       </c>
       <c r="K53" t="n">
-        <v>0.2691040294853204</v>
+        <v>0.2691040294853203</v>
       </c>
       <c r="L53" t="n">
         <v>3</v>
@@ -4057,8 +4057,8 @@
       <c r="P53" t="n">
         <v>0.5746041788589592</v>
       </c>
-      <c r="Q53" t="n">
-        <v>6</v>
+      <c r="Q53" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="R53" t="n">
         <v>1.665693703666284</v>
@@ -4073,18 +4073,18 @@
         <v>0.3926990816987241</v>
       </c>
       <c r="V53" s="1" t="n">
-        <v>1.665693703666284</v>
+        <v>0.8167532188690347</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>0.46556557</v>
+        <v>0.46556556224823</v>
       </c>
       <c r="B54" t="n">
-        <v>0.6170146249999999</v>
-      </c>
-      <c r="C54" t="n">
-        <v>3.496558429027839</v>
+        <v>0.6170146465301514</v>
+      </c>
+      <c r="C54" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D54" t="n">
         <v>8</v>
@@ -4098,8 +4098,8 @@
       <c r="G54" t="n">
         <v>1</v>
       </c>
-      <c r="H54" t="n">
-        <v>15</v>
+      <c r="H54" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="I54" t="n">
         <v>0.1111111111111111</v>
@@ -4125,8 +4125,8 @@
       <c r="P54" t="n">
         <v>0.7815817352682647</v>
       </c>
-      <c r="Q54" t="n">
-        <v>6</v>
+      <c r="Q54" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="R54" t="n">
         <v>1.639934155283393</v>
@@ -4141,18 +4141,18 @@
         <v>0.3926990816987241</v>
       </c>
       <c r="V54" s="1" t="n">
-        <v>1.639934155283393</v>
+        <v>0.6290438955262714</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>0.01569920000000008</v>
+        <v>0.01569919288158417</v>
       </c>
       <c r="B55" t="n">
-        <v>-0.1821102799999999</v>
-      </c>
-      <c r="C55" t="n">
-        <v>2.368973864826367</v>
+        <v>-0.1821102797985077</v>
+      </c>
+      <c r="C55" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="D55" t="n">
         <v>6</v>
@@ -4166,11 +4166,11 @@
       <c r="G55" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H55" t="n">
-        <v>7</v>
-      </c>
-      <c r="I55" t="n">
-        <v>0.08000000000000002</v>
+      <c r="H55" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I55" s="1" t="n">
+        <v>0.02666666666666668</v>
       </c>
       <c r="J55" t="n">
         <v>0</v>
@@ -4193,8 +4193,8 @@
       <c r="P55" t="n">
         <v>0.5265412832179288</v>
       </c>
-      <c r="Q55" t="n">
-        <v>5</v>
+      <c r="Q55" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="R55" t="n">
         <v>1.73023804570537</v>
@@ -4209,18 +4209,18 @@
         <v>0.3926990816987241</v>
       </c>
       <c r="V55" s="1" t="n">
-        <v>1.73023804570537</v>
+        <v>0.9114871685485055</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>0.03023049999999999</v>
+        <v>0.03023050725460052</v>
       </c>
       <c r="B56" t="n">
-        <v>-0.7950617</v>
-      </c>
-      <c r="C56" t="n">
-        <v>2.422027532951638</v>
+        <v>-0.7950617522001266</v>
+      </c>
+      <c r="C56" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="D56" t="n">
         <v>6</v>
@@ -4234,11 +4234,11 @@
       <c r="G56" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H56" t="n">
-        <v>8</v>
-      </c>
-      <c r="I56" t="n">
-        <v>0.08000000000000002</v>
+      <c r="H56" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I56" s="1" t="n">
+        <v>0.04000000000000001</v>
       </c>
       <c r="J56" t="n">
         <v>0</v>
@@ -4261,11 +4261,11 @@
       <c r="P56" t="n">
         <v>0.441599982420937</v>
       </c>
-      <c r="Q56" t="n">
-        <v>5</v>
-      </c>
-      <c r="R56" t="n">
-        <v>1.816271261963039</v>
+      <c r="Q56" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="R56" s="1" t="n">
+        <v>1.778747513382372</v>
       </c>
       <c r="S56" t="n">
         <v>0</v>
@@ -4277,21 +4277,21 @@
         <v>0.5890486225480862</v>
       </c>
       <c r="V56" s="1" t="n">
-        <v>1.816271261963039</v>
+        <v>0.8859659347284118</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>0.67213682</v>
+        <v>0.6721368432044983</v>
       </c>
       <c r="B57" t="n">
-        <v>-0.4745313399999999</v>
-      </c>
-      <c r="C57" t="n">
-        <v>3.60435448385191</v>
-      </c>
-      <c r="D57" t="n">
-        <v>10</v>
+        <v>-0.4745312929153442</v>
+      </c>
+      <c r="C57" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D57" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="E57" t="n">
         <v>0.5506835418044481</v>
@@ -4302,8 +4302,8 @@
       <c r="G57" t="n">
         <v>0.8695652173913043</v>
       </c>
-      <c r="H57" t="n">
-        <v>15</v>
+      <c r="H57" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="I57" t="n">
         <v>0.1111111111111111</v>
@@ -4312,10 +4312,10 @@
         <v>0</v>
       </c>
       <c r="K57" t="n">
-        <v>0.3598252058136452</v>
-      </c>
-      <c r="L57" t="n">
-        <v>5</v>
+        <v>0.3598252058136453</v>
+      </c>
+      <c r="L57" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="M57" t="n">
         <v>0.5</v>
@@ -4329,11 +4329,11 @@
       <c r="P57" t="n">
         <v>0.7750123137142799</v>
       </c>
-      <c r="Q57" t="n">
-        <v>4</v>
+      <c r="Q57" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="R57" t="n">
-        <v>1.790511713580147</v>
+        <v>1.790511713580148</v>
       </c>
       <c r="S57" t="n">
         <v>0</v>
@@ -4345,18 +4345,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V57" s="1" t="n">
-        <v>1.790511713580147</v>
+        <v>0.6330814726579055</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>0.40187351</v>
+        <v>0.4018734991550446</v>
       </c>
       <c r="B58" t="n">
-        <v>-0.621077195</v>
-      </c>
-      <c r="C58" t="n">
-        <v>3.490086255294618</v>
+        <v>-0.621077224612236</v>
+      </c>
+      <c r="C58" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D58" t="n">
         <v>9</v>
@@ -4370,8 +4370,8 @@
       <c r="G58" t="n">
         <v>0.7826086956521739</v>
       </c>
-      <c r="H58" t="n">
-        <v>15</v>
+      <c r="H58" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="I58" t="n">
         <v>0.1111111111111111</v>
@@ -4397,11 +4397,11 @@
       <c r="P58" t="n">
         <v>0.7963553909586716</v>
       </c>
-      <c r="Q58" t="n">
-        <v>6</v>
-      </c>
-      <c r="R58" t="n">
-        <v>1.665693703666284</v>
+      <c r="Q58" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="R58" s="1" t="n">
+        <v>1.73023804570537</v>
       </c>
       <c r="S58" t="n">
         <v>0</v>
@@ -4413,21 +4413,21 @@
         <v>0.3926990816987241</v>
       </c>
       <c r="V58" s="1" t="n">
-        <v>1.665693703666284</v>
+        <v>0.6452642671077279</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>0.8345176099999997</v>
+        <v>0.8345175981521606</v>
       </c>
       <c r="B59" t="n">
-        <v>0.9700087549999996</v>
-      </c>
-      <c r="C59" t="n">
-        <v>3.722507137149014</v>
-      </c>
-      <c r="D59" t="n">
-        <v>14</v>
+        <v>0.9700087308883667</v>
+      </c>
+      <c r="C59" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D59" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="E59" t="n">
         <v>0.6723319593699535</v>
@@ -4438,11 +4438,11 @@
       <c r="G59" t="n">
         <v>1</v>
       </c>
-      <c r="H59" t="n">
-        <v>15</v>
-      </c>
-      <c r="I59" t="n">
-        <v>0.07407407407407407</v>
+      <c r="H59" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I59" s="1" t="n">
+        <v>0.1111111111111111</v>
       </c>
       <c r="J59" t="n">
         <v>0</v>
@@ -4465,11 +4465,11 @@
       <c r="P59" t="n">
         <v>0.7561383689918901</v>
       </c>
-      <c r="Q59" t="n">
-        <v>5</v>
+      <c r="Q59" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="R59" t="n">
-        <v>1.790511713580147</v>
+        <v>1.790511713580148</v>
       </c>
       <c r="S59" t="n">
         <v>0</v>
@@ -4481,18 +4481,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V59" s="1" t="n">
-        <v>1.790511713580147</v>
+        <v>0.5889727405753026</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>-0.44019961</v>
+        <v>-0.4401995986700058</v>
       </c>
       <c r="B60" t="n">
-        <v>-0.1767330864285714</v>
-      </c>
-      <c r="C60" t="n">
-        <v>2.90986616407829</v>
+        <v>-0.1767330850873675</v>
+      </c>
+      <c r="C60" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="D60" t="n">
         <v>6</v>
@@ -4506,8 +4506,8 @@
       <c r="G60" t="n">
         <v>1</v>
       </c>
-      <c r="H60" t="n">
-        <v>5</v>
+      <c r="H60" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="I60" t="n">
         <v>0.1041666666666667</v>
@@ -4533,8 +4533,8 @@
       <c r="P60" t="n">
         <v>0.5371926654867829</v>
       </c>
-      <c r="Q60" t="n">
-        <v>4</v>
+      <c r="Q60" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="R60" t="n">
         <v>1.714203171343286</v>
@@ -4549,18 +4549,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V60" s="1" t="n">
-        <v>1.714203171343286</v>
+        <v>0.7519781333833444</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>-0.27829961</v>
+        <v>-0.2782995998859406</v>
       </c>
       <c r="B61" t="n">
-        <v>-0.456228875</v>
-      </c>
-      <c r="C61" t="n">
-        <v>1.773841537990254</v>
+        <v>-0.4562288522720337</v>
+      </c>
+      <c r="C61" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="D61" t="n">
         <v>6</v>
@@ -4574,8 +4574,8 @@
       <c r="G61" t="n">
         <v>0.9565217391304348</v>
       </c>
-      <c r="H61" t="n">
-        <v>4</v>
+      <c r="H61" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="I61" t="n">
         <v>0.03401360544217687</v>
@@ -4584,7 +4584,7 @@
         <v>0</v>
       </c>
       <c r="K61" t="n">
-        <v>0.09378303137176296</v>
+        <v>0.09378303137176291</v>
       </c>
       <c r="L61" t="n">
         <v>2</v>
@@ -4601,8 +4601,8 @@
       <c r="P61" t="n">
         <v>0.2440544779975879</v>
       </c>
-      <c r="Q61" t="n">
-        <v>5</v>
+      <c r="Q61" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="R61" t="n">
         <v>1.885299500946812</v>
@@ -4617,21 +4617,21 @@
         <v>0.5890486225480862</v>
       </c>
       <c r="V61" s="1" t="n">
-        <v>1.885299500946812</v>
+        <v>0.8507203206479008</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>1.04530324</v>
+        <v>1.045303225517273</v>
       </c>
       <c r="B62" t="n">
-        <v>-1.37903582</v>
-      </c>
-      <c r="C62" t="n">
-        <v>3.622396088656317</v>
-      </c>
-      <c r="D62" t="n">
-        <v>9</v>
+        <v>-1.379035830497742</v>
+      </c>
+      <c r="C62" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D62" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="E62" t="n">
         <v>0.7052684720641098</v>
@@ -4642,8 +4642,8 @@
       <c r="G62" t="n">
         <v>0.8695652173913043</v>
       </c>
-      <c r="H62" t="n">
-        <v>13</v>
+      <c r="H62" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="I62" t="n">
         <v>0.1111111111111111</v>
@@ -4669,8 +4669,8 @@
       <c r="P62" t="n">
         <v>0.8388125180040888</v>
       </c>
-      <c r="Q62" t="n">
-        <v>6</v>
+      <c r="Q62" s="1" t="n">
+        <v>13</v>
       </c>
       <c r="R62" t="n">
         <v>1.483611654966423</v>
@@ -4685,21 +4685,21 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V62" s="1" t="n">
-        <v>1.483611654966423</v>
+        <v>0.6376839124264988</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>0.8659695499999998</v>
+        <v>0.8659695386886597</v>
       </c>
       <c r="B63" t="n">
-        <v>1.000827175</v>
-      </c>
-      <c r="C63" t="n">
-        <v>3.581393477539761</v>
-      </c>
-      <c r="D63" t="n">
-        <v>14</v>
+        <v>1.000827193260193</v>
+      </c>
+      <c r="C63" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D63" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="E63" t="n">
         <v>0.6406273588011022</v>
@@ -4710,11 +4710,11 @@
       <c r="G63" t="n">
         <v>0.8260869565217391</v>
       </c>
-      <c r="H63" t="n">
-        <v>15</v>
-      </c>
-      <c r="I63" t="n">
-        <v>0.07407407407407407</v>
+      <c r="H63" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="I63" s="1" t="n">
+        <v>0.1111111111111111</v>
       </c>
       <c r="J63" t="n">
         <v>0</v>
@@ -4737,8 +4737,8 @@
       <c r="P63" t="n">
         <v>0.7348060490043172</v>
       </c>
-      <c r="Q63" t="n">
-        <v>5</v>
+      <c r="Q63" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="R63" t="n">
         <v>1.73023804570537</v>
@@ -4753,18 +4753,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V63" s="1" t="n">
-        <v>1.73023804570537</v>
+        <v>0.6135343276114881</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>0.6499297199999998</v>
+        <v>0.6499297171831131</v>
       </c>
       <c r="B64" t="n">
-        <v>1.07429208</v>
-      </c>
-      <c r="C64" t="n">
-        <v>3.153595860988778</v>
+        <v>1.074292063713074</v>
+      </c>
+      <c r="C64" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D64" t="n">
         <v>7</v>
@@ -4778,8 +4778,8 @@
       <c r="G64" t="n">
         <v>0.7826086956521739</v>
       </c>
-      <c r="H64" t="n">
-        <v>15</v>
+      <c r="H64" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="I64" t="n">
         <v>0.0625</v>
@@ -4805,11 +4805,11 @@
       <c r="P64" t="n">
         <v>0.6688431671727501</v>
       </c>
-      <c r="Q64" t="n">
-        <v>6</v>
-      </c>
-      <c r="R64" t="n">
-        <v>1.730238045705369</v>
+      <c r="Q64" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="R64" s="1" t="n">
+        <v>1.790511713580148</v>
       </c>
       <c r="S64" t="n">
         <v>0</v>
@@ -4821,18 +4821,18 @@
         <v>0.3926990816987241</v>
       </c>
       <c r="V64" s="1" t="n">
-        <v>1.730238045705369</v>
+        <v>0.7125797158656658</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>1.00578978</v>
+        <v>1.005789756774902</v>
       </c>
       <c r="B65" t="n">
-        <v>0.8525265699999998</v>
-      </c>
-      <c r="C65" t="n">
-        <v>3.412585659954937</v>
+        <v>0.8525265455245972</v>
+      </c>
+      <c r="C65" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D65" t="n">
         <v>8</v>
@@ -4846,8 +4846,8 @@
       <c r="G65" t="n">
         <v>1</v>
       </c>
-      <c r="H65" t="n">
-        <v>12</v>
+      <c r="H65" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="I65" t="n">
         <v>0.1111111111111111</v>
@@ -4873,11 +4873,11 @@
       <c r="P65" t="n">
         <v>0.728706648937482</v>
       </c>
-      <c r="Q65" t="n">
-        <v>5</v>
-      </c>
-      <c r="R65" t="n">
-        <v>1.857500426386953</v>
+      <c r="Q65" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="R65" s="1" t="n">
+        <v>1.665693703666284</v>
       </c>
       <c r="S65" t="n">
         <v>0</v>
@@ -4889,21 +4889,21 @@
         <v>0.3926990816987241</v>
       </c>
       <c r="V65" s="1" t="n">
-        <v>1.857500426386953</v>
+        <v>0.6997252821898771</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>0.8993800099999999</v>
+        <v>0.8993799686431885</v>
       </c>
       <c r="B66" t="n">
-        <v>0.760180165</v>
-      </c>
-      <c r="C66" t="n">
-        <v>3.458975349733846</v>
-      </c>
-      <c r="D66" t="n">
-        <v>9</v>
+        <v>0.7601801753044128</v>
+      </c>
+      <c r="C66" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D66" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="E66" t="n">
         <v>0.6521124287654525</v>
@@ -4914,11 +4914,11 @@
       <c r="G66" t="n">
         <v>0.9565217391304348</v>
       </c>
-      <c r="H66" t="n">
-        <v>16</v>
-      </c>
-      <c r="I66" t="n">
-        <v>0.07407407407407407</v>
+      <c r="H66" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="I66" s="1" t="n">
+        <v>0.1111111111111111</v>
       </c>
       <c r="J66" t="n">
         <v>0</v>
@@ -4941,8 +4941,8 @@
       <c r="P66" t="n">
         <v>0.7478701909544907</v>
       </c>
-      <c r="Q66" t="n">
-        <v>7</v>
+      <c r="Q66" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="R66" t="n">
         <v>1.73023804570537</v>
@@ -4957,18 +4957,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V66" s="1" t="n">
-        <v>1.73023804570537</v>
+        <v>0.6442363093792414</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>-1.21779917</v>
+        <v>-1.217799186706543</v>
       </c>
       <c r="B67" t="n">
-        <v>-1.362041885</v>
-      </c>
-      <c r="C67" t="n">
-        <v>3.654000422760018</v>
+        <v>-1.36204195022583</v>
+      </c>
+      <c r="C67" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="D67" t="n">
         <v>9</v>
@@ -4982,8 +4982,8 @@
       <c r="G67" t="n">
         <v>0.9130434782608695</v>
       </c>
-      <c r="H67" t="n">
-        <v>14</v>
+      <c r="H67" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="I67" t="n">
         <v>0.1111111111111111</v>
@@ -5009,8 +5009,8 @@
       <c r="P67" t="n">
         <v>0.812657865345757</v>
       </c>
-      <c r="Q67" t="n">
-        <v>6</v>
+      <c r="Q67" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="R67" t="n">
         <v>1.665693703666284</v>
@@ -5025,18 +5025,18 @@
         <v>0.1963495408493621</v>
       </c>
       <c r="V67" s="1" t="n">
-        <v>1.665693703666284</v>
+        <v>0.6439677083574314</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>-0.51315894</v>
+        <v>-0.513158917427063</v>
       </c>
       <c r="B68" t="n">
-        <v>-0.7230163999999999</v>
-      </c>
-      <c r="C68" t="n">
-        <v>1.748013550088016</v>
+        <v>-0.7230163812637329</v>
+      </c>
+      <c r="C68" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="D68" t="n">
         <v>6</v>
@@ -5060,7 +5060,7 @@
         <v>0</v>
       </c>
       <c r="K68" t="n">
-        <v>0.09001035183246438</v>
+        <v>0.09001035183246436</v>
       </c>
       <c r="L68" t="n">
         <v>2</v>
@@ -5080,8 +5080,8 @@
       <c r="Q68" t="n">
         <v>6</v>
       </c>
-      <c r="R68" t="n">
-        <v>1.831740878004061</v>
+      <c r="R68" s="1" t="n">
+        <v>1.847775752366145</v>
       </c>
       <c r="S68" t="n">
         <v>0</v>
@@ -5093,7 +5093,7 @@
         <v>0.5890486225480862</v>
       </c>
       <c r="V68" s="1" t="n">
-        <v>1.831740878004061</v>
+        <v>0.9414478639673471</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reverted changes before zero division error as issues were caused + new errors found that need to be fixed first
</commit_message>
<xml_diff>
--- a/tsml_eval/_wip/catch22/aeon_catch22_with_numba.xlsx
+++ b/tsml_eval/_wip/catch22/aeon_catch22_with_numba.xlsx
@@ -547,8 +547,8 @@
       <c r="B2" t="n">
         <v>-0.73655276</v>
       </c>
-      <c r="C2" s="1" t="n">
-        <v>21.25829518192415</v>
+      <c r="C2" t="n">
+        <v>17.40819215506482</v>
       </c>
       <c r="D2" t="n">
         <v>50</v>
@@ -565,8 +565,8 @@
       <c r="H2" t="n">
         <v>61</v>
       </c>
-      <c r="I2" s="1" t="n">
-        <v>0.005208333333333334</v>
+      <c r="I2" t="n">
+        <v>0.02057613168724279</v>
       </c>
       <c r="J2" t="n">
         <v>74</v>
@@ -578,7 +578,7 @@
         <v>24</v>
       </c>
       <c r="M2" s="1" t="n">
-        <v>0.9333333333333333</v>
+        <v>1.076923076923077</v>
       </c>
       <c r="N2" t="n">
         <v>0.007968127490039823</v>
@@ -615,8 +615,8 @@
       <c r="B3" t="n">
         <v>1.181283415</v>
       </c>
-      <c r="C3" s="1" t="n">
-        <v>23.5051996518466</v>
+      <c r="C3" t="n">
+        <v>19.91810114448176</v>
       </c>
       <c r="D3" t="n">
         <v>60</v>
@@ -633,8 +633,8 @@
       <c r="H3" t="n">
         <v>69</v>
       </c>
-      <c r="I3" s="1" t="n">
-        <v>0.01360544217687075</v>
+      <c r="I3" t="n">
+        <v>0.03645833333333334</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
@@ -646,7 +646,7 @@
         <v>28</v>
       </c>
       <c r="M3" s="1" t="n">
-        <v>1</v>
+        <v>1.066666666666667</v>
       </c>
       <c r="N3" t="n">
         <v>0.2868525896414342</v>
@@ -683,8 +683,8 @@
       <c r="B4" t="n">
         <v>1.262308135</v>
       </c>
-      <c r="C4" s="1" t="n">
-        <v>22.75218522235674</v>
+      <c r="C4" t="n">
+        <v>19.12800902518529</v>
       </c>
       <c r="D4" t="n">
         <v>60</v>
@@ -701,8 +701,8 @@
       <c r="H4" t="n">
         <v>65</v>
       </c>
-      <c r="I4" s="1" t="n">
-        <v>0.01360544217687075</v>
+      <c r="I4" t="n">
+        <v>0.03645833333333334</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
@@ -714,7 +714,7 @@
         <v>27</v>
       </c>
       <c r="M4" s="1" t="n">
-        <v>0.90625</v>
+        <v>1</v>
       </c>
       <c r="N4" s="1" t="n">
         <v>-0.3984063745019921</v>
@@ -751,8 +751,8 @@
       <c r="B5" t="n">
         <v>-0.02298369500000019</v>
       </c>
-      <c r="C5" s="1" t="n">
-        <v>19.17232033763232</v>
+      <c r="C5" t="n">
+        <v>15.74855722832491</v>
       </c>
       <c r="D5" t="n">
         <v>43</v>
@@ -769,20 +769,20 @@
       <c r="H5" t="n">
         <v>57</v>
       </c>
-      <c r="I5" s="1" t="n">
-        <v>0.02083333333333334</v>
+      <c r="I5" t="n">
+        <v>0.05333333333333334</v>
       </c>
       <c r="J5" t="n">
         <v>72</v>
       </c>
-      <c r="K5" s="1" t="n">
-        <v>3.801556777207852</v>
+      <c r="K5" t="n">
+        <v>3.485826843761838</v>
       </c>
       <c r="L5" t="n">
         <v>22</v>
       </c>
       <c r="M5" s="1" t="n">
-        <v>0.8928571428571429</v>
+        <v>1.041666666666667</v>
       </c>
       <c r="N5" t="n">
         <v>0.4661354581673307</v>
@@ -819,8 +819,8 @@
       <c r="B6" t="n">
         <v>-0.9409232250000001</v>
       </c>
-      <c r="C6" s="1" t="n">
-        <v>23.17864643630214</v>
+      <c r="C6" t="n">
+        <v>19.60514228209162</v>
       </c>
       <c r="D6" t="n">
         <v>56</v>
@@ -837,8 +837,8 @@
       <c r="H6" t="n">
         <v>66</v>
       </c>
-      <c r="I6" s="1" t="n">
-        <v>0.01360544217687075</v>
+      <c r="I6" t="n">
+        <v>0.03645833333333334</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
@@ -850,7 +850,7 @@
         <v>27</v>
       </c>
       <c r="M6" s="1" t="n">
-        <v>1.03125</v>
+        <v>1.137931034482759</v>
       </c>
       <c r="N6" t="n">
         <v>-0.2589641434262948</v>
@@ -887,8 +887,8 @@
       <c r="B7" t="n">
         <v>1.106436265</v>
       </c>
-      <c r="C7" s="1" t="n">
-        <v>22.77321453569093</v>
+      <c r="C7" t="n">
+        <v>18.25902148010383</v>
       </c>
       <c r="D7" t="n">
         <v>63</v>
@@ -905,8 +905,8 @@
       <c r="H7" t="n">
         <v>74</v>
       </c>
-      <c r="I7" s="1" t="n">
-        <v>0.01360544217687075</v>
+      <c r="I7" t="n">
+        <v>0.03645833333333334</v>
       </c>
       <c r="J7" t="n">
         <v>28</v>
@@ -918,7 +918,7 @@
         <v>27</v>
       </c>
       <c r="M7" s="1" t="n">
-        <v>1.03125</v>
+        <v>1.137931034482759</v>
       </c>
       <c r="N7" s="1" t="n">
         <v>-0.003984063745019938</v>
@@ -955,8 +955,8 @@
       <c r="B8" t="n">
         <v>0.3369372949999999</v>
       </c>
-      <c r="C8" s="1" t="n">
-        <v>18.68492342084755</v>
+      <c r="C8" t="n">
+        <v>15.07024562620989</v>
       </c>
       <c r="D8" t="n">
         <v>44</v>
@@ -973,20 +973,20 @@
       <c r="H8" t="n">
         <v>60</v>
       </c>
-      <c r="I8" s="1" t="n">
-        <v>0.03645833333333334</v>
+      <c r="I8" t="n">
+        <v>0.05333333333333334</v>
       </c>
       <c r="J8" t="n">
         <v>71</v>
       </c>
-      <c r="K8" s="1" t="n">
-        <v>3.059792363763536</v>
+      <c r="K8" t="n">
+        <v>3.205331201526457</v>
       </c>
       <c r="L8" t="n">
         <v>22</v>
       </c>
       <c r="M8" s="1" t="n">
-        <v>1</v>
+        <v>1.166666666666667</v>
       </c>
       <c r="N8" t="n">
         <v>0.4780876494023904</v>
@@ -1023,8 +1023,8 @@
       <c r="B9" t="n">
         <v>1.343709465</v>
       </c>
-      <c r="C9" s="1" t="n">
-        <v>23.34773840644704</v>
+      <c r="C9" t="n">
+        <v>19.87341873939329</v>
       </c>
       <c r="D9" t="n">
         <v>56</v>
@@ -1041,8 +1041,8 @@
       <c r="H9" t="n">
         <v>65</v>
       </c>
-      <c r="I9" s="1" t="n">
-        <v>0.01360544217687075</v>
+      <c r="I9" t="n">
+        <v>0.03645833333333334</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
@@ -1054,7 +1054,7 @@
         <v>27</v>
       </c>
       <c r="M9" s="1" t="n">
-        <v>1.060606060606061</v>
+        <v>1.206896551724138</v>
       </c>
       <c r="N9" t="n">
         <v>0.2430278884462151</v>
@@ -1091,8 +1091,8 @@
       <c r="B10" t="n">
         <v>1.16609466</v>
       </c>
-      <c r="C10" s="1" t="n">
-        <v>23.29716070307969</v>
+      <c r="C10" t="n">
+        <v>19.8912023015621</v>
       </c>
       <c r="D10" t="n">
         <v>61</v>
@@ -1109,8 +1109,8 @@
       <c r="H10" t="n">
         <v>67</v>
       </c>
-      <c r="I10" s="1" t="n">
-        <v>0.01360544217687075</v>
+      <c r="I10" t="n">
+        <v>0.03645833333333334</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
@@ -1122,7 +1122,7 @@
         <v>28</v>
       </c>
       <c r="M10" s="1" t="n">
-        <v>0.96875</v>
+        <v>1.033333333333333</v>
       </c>
       <c r="N10" t="n">
         <v>0.003984063745019903</v>
@@ -1159,8 +1159,8 @@
       <c r="B11" t="n">
         <v>0.2233287800000001</v>
       </c>
-      <c r="C11" s="1" t="n">
-        <v>17.38347922591631</v>
+      <c r="C11" t="n">
+        <v>13.95569405639475</v>
       </c>
       <c r="D11" t="n">
         <v>42</v>
@@ -1177,20 +1177,20 @@
       <c r="H11" t="n">
         <v>60</v>
       </c>
-      <c r="I11" s="1" t="n">
-        <v>0.008230452674897118</v>
+      <c r="I11" t="n">
+        <v>0.03856749311294766</v>
       </c>
       <c r="J11" t="n">
         <v>79</v>
       </c>
-      <c r="K11" s="1" t="n">
-        <v>3.048535231242921</v>
+      <c r="K11" t="n">
+        <v>3.447937982072726</v>
       </c>
       <c r="L11" t="n">
         <v>20</v>
       </c>
       <c r="M11" s="1" t="n">
-        <v>0.8846153846153846</v>
+        <v>1.045454545454545</v>
       </c>
       <c r="N11" t="n">
         <v>0.3784860557768924</v>
@@ -1227,8 +1227,8 @@
       <c r="B12" t="n">
         <v>1.02353097</v>
       </c>
-      <c r="C12" s="1" t="n">
-        <v>23.27421265839473</v>
+      <c r="C12" t="n">
+        <v>19.31401097013146</v>
       </c>
       <c r="D12" t="n">
         <v>62</v>
@@ -1245,8 +1245,8 @@
       <c r="H12" t="n">
         <v>72</v>
       </c>
-      <c r="I12" s="1" t="n">
-        <v>0.01360544217687075</v>
+      <c r="I12" t="n">
+        <v>0.03645833333333334</v>
       </c>
       <c r="J12" t="n">
         <v>0</v>
@@ -1258,7 +1258,7 @@
         <v>28</v>
       </c>
       <c r="M12" s="1" t="n">
-        <v>0.96875</v>
+        <v>1.033333333333333</v>
       </c>
       <c r="N12" t="n">
         <v>-1.734723475976807e-17</v>
@@ -1295,8 +1295,8 @@
       <c r="B13" t="n">
         <v>1.27095891</v>
       </c>
-      <c r="C13" s="1" t="n">
-        <v>22.40284563464613</v>
+      <c r="C13" t="n">
+        <v>18.77543457306755</v>
       </c>
       <c r="D13" t="n">
         <v>62</v>
@@ -1313,8 +1313,8 @@
       <c r="H13" t="n">
         <v>68</v>
       </c>
-      <c r="I13" s="1" t="n">
-        <v>0.01360544217687075</v>
+      <c r="I13" t="n">
+        <v>0.005208333333333334</v>
       </c>
       <c r="J13" t="n">
         <v>47</v>
@@ -1326,7 +1326,7 @@
         <v>27</v>
       </c>
       <c r="M13" s="1" t="n">
-        <v>0.90625</v>
+        <v>1</v>
       </c>
       <c r="N13" t="n">
         <v>0.2848605577689243</v>
@@ -1363,8 +1363,8 @@
       <c r="B14" t="n">
         <v>-0.01614573499999966</v>
       </c>
-      <c r="C14" s="1" t="n">
-        <v>18.46614051112804</v>
+      <c r="C14" t="n">
+        <v>14.71971926437311</v>
       </c>
       <c r="D14" t="n">
         <v>44</v>
@@ -1381,20 +1381,20 @@
       <c r="H14" t="n">
         <v>57</v>
       </c>
-      <c r="I14" s="1" t="n">
-        <v>0.03645833333333334</v>
+      <c r="I14" t="n">
+        <v>0.05333333333333334</v>
       </c>
       <c r="J14" t="n">
         <v>70</v>
       </c>
-      <c r="K14" s="1" t="n">
-        <v>2.759015910992664</v>
+      <c r="K14" t="n">
+        <v>2.763424943782517</v>
       </c>
       <c r="L14" t="n">
         <v>22</v>
       </c>
       <c r="M14" s="1" t="n">
-        <v>0.8214285714285714</v>
+        <v>0.9583333333333334</v>
       </c>
       <c r="N14" t="n">
         <v>0.4023904382470119</v>
@@ -1431,8 +1431,8 @@
       <c r="B15" t="n">
         <v>1.13672633</v>
       </c>
-      <c r="C15" s="1" t="n">
-        <v>23.46519446305943</v>
+      <c r="C15" t="n">
+        <v>19.47582887855932</v>
       </c>
       <c r="D15" t="n">
         <v>61</v>
@@ -1449,8 +1449,8 @@
       <c r="H15" t="n">
         <v>66</v>
       </c>
-      <c r="I15" s="1" t="n">
-        <v>0.01360544217687075</v>
+      <c r="I15" t="n">
+        <v>0.03645833333333334</v>
       </c>
       <c r="J15" t="n">
         <v>0</v>
@@ -1462,7 +1462,7 @@
         <v>28</v>
       </c>
       <c r="M15" s="1" t="n">
-        <v>1</v>
+        <v>1.066666666666667</v>
       </c>
       <c r="N15" t="n">
         <v>0.007968127490039823</v>
@@ -1499,8 +1499,8 @@
       <c r="B16" t="n">
         <v>0.7245889299999998</v>
       </c>
-      <c r="C16" s="1" t="n">
-        <v>19.85470607659734</v>
+      <c r="C16" t="n">
+        <v>15.05564418777329</v>
       </c>
       <c r="D16" t="n">
         <v>53</v>
@@ -1517,8 +1517,8 @@
       <c r="H16" t="n">
         <v>78</v>
       </c>
-      <c r="I16" s="1" t="n">
-        <v>0.01360544217687075</v>
+      <c r="I16" t="n">
+        <v>0.02057613168724279</v>
       </c>
       <c r="J16" t="n">
         <v>61</v>
@@ -1530,7 +1530,7 @@
         <v>24</v>
       </c>
       <c r="M16" s="1" t="n">
-        <v>0.5</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="N16" t="n">
         <v>0.2430278884462151</v>
@@ -1567,8 +1567,8 @@
       <c r="B17" t="n">
         <v>0.6968899499999999</v>
       </c>
-      <c r="C17" s="1" t="n">
-        <v>16.80081026109782</v>
+      <c r="C17" t="n">
+        <v>13.60061437498968</v>
       </c>
       <c r="D17" t="n">
         <v>42</v>
@@ -1585,20 +1585,20 @@
       <c r="H17" t="n">
         <v>52</v>
       </c>
-      <c r="I17" s="1" t="n">
-        <v>0.01333333333333333</v>
+      <c r="I17" t="n">
+        <v>0.04683195592286502</v>
       </c>
       <c r="J17" t="n">
         <v>70</v>
       </c>
-      <c r="K17" s="1" t="n">
-        <v>2.35765325305948</v>
+      <c r="K17" t="n">
+        <v>2.269837011114737</v>
       </c>
       <c r="L17" t="n">
         <v>20</v>
       </c>
-      <c r="M17" s="1" t="n">
-        <v>0.88</v>
+      <c r="M17" t="n">
+        <v>1</v>
       </c>
       <c r="N17" t="n">
         <v>-0.0159362549800797</v>
@@ -1635,8 +1635,8 @@
       <c r="B18" t="n">
         <v>0.8744098100000004</v>
       </c>
-      <c r="C18" s="1" t="n">
-        <v>22.36555561067515</v>
+      <c r="C18" t="n">
+        <v>18.13592238629358</v>
       </c>
       <c r="D18" t="n">
         <v>65</v>
@@ -1653,8 +1653,8 @@
       <c r="H18" t="n">
         <v>75</v>
       </c>
-      <c r="I18" s="1" t="n">
-        <v>0.03645833333333334</v>
+      <c r="I18" t="n">
+        <v>0.02083333333333333</v>
       </c>
       <c r="J18" t="n">
         <v>0</v>
@@ -1666,7 +1666,7 @@
         <v>27</v>
       </c>
       <c r="M18" s="1" t="n">
-        <v>0.8387096774193549</v>
+        <v>0.896551724137931</v>
       </c>
       <c r="N18" t="n">
         <v>0.01195219123505974</v>
@@ -1703,8 +1703,8 @@
       <c r="B19" t="n">
         <v>1.075372055</v>
       </c>
-      <c r="C19" s="1" t="n">
-        <v>23.34297969593479</v>
+      <c r="C19" t="n">
+        <v>20.3637157720036</v>
       </c>
       <c r="D19" t="n">
         <v>61</v>
@@ -1721,8 +1721,8 @@
       <c r="H19" t="n">
         <v>72</v>
       </c>
-      <c r="I19" s="1" t="n">
-        <v>0.01360544217687075</v>
+      <c r="I19" t="n">
+        <v>0.03645833333333334</v>
       </c>
       <c r="J19" t="n">
         <v>0</v>
@@ -1734,7 +1734,7 @@
         <v>28</v>
       </c>
       <c r="M19" s="1" t="n">
-        <v>0.96875</v>
+        <v>1.033333333333333</v>
       </c>
       <c r="N19" t="n">
         <v>0.007968127490039823</v>
@@ -1771,8 +1771,8 @@
       <c r="B20" t="n">
         <v>1.317673195</v>
       </c>
-      <c r="C20" s="1" t="n">
-        <v>19.27624130653107</v>
+      <c r="C20" t="n">
+        <v>15.62873760559645</v>
       </c>
       <c r="D20" t="n">
         <v>43</v>
@@ -1789,20 +1789,20 @@
       <c r="H20" t="n">
         <v>59</v>
       </c>
-      <c r="I20" s="1" t="n">
-        <v>0.02083333333333334</v>
+      <c r="I20" t="n">
+        <v>0.05333333333333334</v>
       </c>
       <c r="J20" t="n">
         <v>70</v>
       </c>
-      <c r="K20" s="1" t="n">
-        <v>3.018923796371801</v>
+      <c r="K20" t="n">
+        <v>2.983229197536327</v>
       </c>
       <c r="L20" t="n">
         <v>22</v>
       </c>
       <c r="M20" s="1" t="n">
-        <v>0.7857142857142857</v>
+        <v>0.9166666666666666</v>
       </c>
       <c r="N20" t="n">
         <v>0.3784860557768924</v>
@@ -1839,8 +1839,8 @@
       <c r="B21" t="n">
         <v>1.089911645</v>
       </c>
-      <c r="C21" s="1" t="n">
-        <v>23.4224444068253</v>
+      <c r="C21" t="n">
+        <v>19.53596071976449</v>
       </c>
       <c r="D21" t="n">
         <v>62</v>
@@ -1857,8 +1857,8 @@
       <c r="H21" t="n">
         <v>68</v>
       </c>
-      <c r="I21" s="1" t="n">
-        <v>0.01360544217687075</v>
+      <c r="I21" t="n">
+        <v>0.03645833333333334</v>
       </c>
       <c r="J21" t="n">
         <v>0</v>
@@ -1870,7 +1870,7 @@
         <v>28</v>
       </c>
       <c r="M21" s="1" t="n">
-        <v>0.96875</v>
+        <v>1.033333333333333</v>
       </c>
       <c r="N21" t="n">
         <v>-0.2609561752988048</v>
@@ -1907,8 +1907,8 @@
       <c r="B22" t="n">
         <v>-0.7275711100000002</v>
       </c>
-      <c r="C22" s="1" t="n">
-        <v>20.73779328904098</v>
+      <c r="C22" t="n">
+        <v>17.21209395200373</v>
       </c>
       <c r="D22" t="n">
         <v>52</v>
@@ -1925,8 +1925,8 @@
       <c r="H22" t="n">
         <v>60</v>
       </c>
-      <c r="I22" s="1" t="n">
-        <v>0.005208333333333334</v>
+      <c r="I22" t="n">
+        <v>0.02057613168724279</v>
       </c>
       <c r="J22" t="n">
         <v>74</v>
@@ -1938,7 +1938,7 @@
         <v>24</v>
       </c>
       <c r="M22" s="1" t="n">
-        <v>0.9</v>
+        <v>1.038461538461539</v>
       </c>
       <c r="N22" t="n">
         <v>0.4541832669322709</v>
@@ -1975,8 +1975,8 @@
       <c r="B23" t="n">
         <v>-0.7294772750000003</v>
       </c>
-      <c r="C23" s="1" t="n">
-        <v>21.2890808926852</v>
+      <c r="C23" t="n">
+        <v>16.82955425677702</v>
       </c>
       <c r="D23" t="n">
         <v>48</v>
@@ -1993,8 +1993,8 @@
       <c r="H23" t="n">
         <v>56</v>
       </c>
-      <c r="I23" s="1" t="n">
-        <v>0.01360544217687075</v>
+      <c r="I23" t="n">
+        <v>0.02083333333333333</v>
       </c>
       <c r="J23" s="1" t="n">
         <v>65</v>
@@ -2006,7 +2006,7 @@
         <v>26</v>
       </c>
       <c r="M23" s="1" t="n">
-        <v>0.46875</v>
+        <v>0.5357142857142857</v>
       </c>
       <c r="N23" t="n">
         <v>0.3605577689243027</v>
@@ -2043,8 +2043,8 @@
       <c r="B24" t="n">
         <v>-0.9515455749999999</v>
       </c>
-      <c r="C24" s="1" t="n">
-        <v>22.5490963165729</v>
+      <c r="C24" t="n">
+        <v>19.11706532842858</v>
       </c>
       <c r="D24" t="n">
         <v>56</v>
@@ -2061,8 +2061,8 @@
       <c r="H24" t="n">
         <v>64</v>
       </c>
-      <c r="I24" s="1" t="n">
-        <v>0.01360544217687075</v>
+      <c r="I24" t="n">
+        <v>0.02083333333333333</v>
       </c>
       <c r="J24" t="n">
         <v>79</v>
@@ -2074,7 +2074,7 @@
         <v>26</v>
       </c>
       <c r="M24" s="1" t="n">
-        <v>1</v>
+        <v>1.142857142857143</v>
       </c>
       <c r="N24" t="n">
         <v>-0.3067729083665339</v>
@@ -2111,8 +2111,8 @@
       <c r="B25" t="n">
         <v>-0.04728045</v>
       </c>
-      <c r="C25" s="1" t="n">
-        <v>16.07337468944941</v>
+      <c r="C25" t="n">
+        <v>12.81366767882287</v>
       </c>
       <c r="D25" t="n">
         <v>47</v>
@@ -2129,20 +2129,20 @@
       <c r="H25" t="n">
         <v>42</v>
       </c>
-      <c r="I25" s="1" t="n">
-        <v>0.04629629629629629</v>
+      <c r="I25" t="n">
+        <v>0.01333333333333333</v>
       </c>
       <c r="J25" t="n">
         <v>70</v>
       </c>
-      <c r="K25" s="1" t="n">
-        <v>2.349693635395747</v>
+      <c r="K25" t="n">
+        <v>2.368434805890583</v>
       </c>
       <c r="L25" t="n">
         <v>21</v>
       </c>
-      <c r="M25" s="1" t="n">
-        <v>0.2894736842105263</v>
+      <c r="M25" t="n">
+        <v>0.4583333333333333</v>
       </c>
       <c r="N25" t="n">
         <v>0.2031872509960159</v>
@@ -2179,8 +2179,8 @@
       <c r="B26" t="n">
         <v>0.004780390000000079</v>
       </c>
-      <c r="C26" s="1" t="n">
-        <v>18.21537414099297</v>
+      <c r="C26" t="n">
+        <v>14.78490457790944</v>
       </c>
       <c r="D26" t="n">
         <v>43</v>
@@ -2197,20 +2197,20 @@
       <c r="H26" t="n">
         <v>58</v>
       </c>
-      <c r="I26" s="1" t="n">
-        <v>0.008230452674897118</v>
+      <c r="I26" t="n">
+        <v>0.02333333333333333</v>
       </c>
       <c r="J26" t="n">
         <v>75</v>
       </c>
-      <c r="K26" s="1" t="n">
-        <v>3.45978718659969</v>
+      <c r="K26" t="n">
+        <v>3.519394837090817</v>
       </c>
       <c r="L26" t="n">
         <v>21</v>
       </c>
       <c r="M26" s="1" t="n">
-        <v>0.9259259259259259</v>
+        <v>1.08695652173913</v>
       </c>
       <c r="N26" t="n">
         <v>0.49800796812749</v>
@@ -2247,8 +2247,8 @@
       <c r="B27" t="n">
         <v>-0.8504074</v>
       </c>
-      <c r="C27" s="1" t="n">
-        <v>23.31035407400848</v>
+      <c r="C27" t="n">
+        <v>20.0659061787455</v>
       </c>
       <c r="D27" t="n">
         <v>57</v>
@@ -2265,8 +2265,8 @@
       <c r="H27" t="n">
         <v>65</v>
       </c>
-      <c r="I27" s="1" t="n">
-        <v>0.01360544217687075</v>
+      <c r="I27" t="n">
+        <v>0.03645833333333334</v>
       </c>
       <c r="J27" t="n">
         <v>0</v>
@@ -2278,7 +2278,7 @@
         <v>27</v>
       </c>
       <c r="M27" s="1" t="n">
-        <v>1.03125</v>
+        <v>1.137931034482759</v>
       </c>
       <c r="N27" t="n">
         <v>-1.734723475976807e-17</v>
@@ -2315,8 +2315,8 @@
       <c r="B28" t="n">
         <v>-0.195689835</v>
       </c>
-      <c r="C28" s="1" t="n">
-        <v>17.86044834467204</v>
+      <c r="C28" t="n">
+        <v>13.65491720725454</v>
       </c>
       <c r="D28" t="n">
         <v>41</v>
@@ -2333,20 +2333,20 @@
       <c r="H28" t="n">
         <v>50</v>
       </c>
-      <c r="I28" s="1" t="n">
-        <v>0.03645833333333333</v>
+      <c r="I28" t="n">
+        <v>0.04333333333333335</v>
       </c>
       <c r="J28" t="n">
         <v>66</v>
       </c>
-      <c r="K28" s="1" t="n">
-        <v>3.620658623103494</v>
+      <c r="K28" t="n">
+        <v>3.707835569091639</v>
       </c>
       <c r="L28" t="n">
         <v>21</v>
       </c>
       <c r="M28" s="1" t="n">
-        <v>1.035714285714286</v>
+        <v>1.260869565217391</v>
       </c>
       <c r="N28" t="n">
         <v>-0.4741035856573705</v>
@@ -2383,8 +2383,8 @@
       <c r="B29" t="n">
         <v>-0.1907815500000001</v>
       </c>
-      <c r="C29" s="1" t="n">
-        <v>23.05889129920445</v>
+      <c r="C29" t="n">
+        <v>18.84136784189097</v>
       </c>
       <c r="D29" t="n">
         <v>57</v>
@@ -2401,8 +2401,8 @@
       <c r="H29" t="n">
         <v>69</v>
       </c>
-      <c r="I29" s="1" t="n">
-        <v>0.01360544217687075</v>
+      <c r="I29" t="n">
+        <v>0.03645833333333334</v>
       </c>
       <c r="J29" t="n">
         <v>0</v>
@@ -2414,7 +2414,7 @@
         <v>27</v>
       </c>
       <c r="M29" s="1" t="n">
-        <v>1.03030303030303</v>
+        <v>1.172413793103448</v>
       </c>
       <c r="N29" t="n">
         <v>0.007968127490039823</v>
@@ -2451,8 +2451,8 @@
       <c r="B30" t="n">
         <v>1.074688215</v>
       </c>
-      <c r="C30" s="1" t="n">
-        <v>23.0433849081225</v>
+      <c r="C30" t="n">
+        <v>18.34457096166117</v>
       </c>
       <c r="D30" t="n">
         <v>61</v>
@@ -2469,8 +2469,8 @@
       <c r="H30" t="n">
         <v>64</v>
       </c>
-      <c r="I30" s="1" t="n">
-        <v>0.01360544217687075</v>
+      <c r="I30" t="n">
+        <v>0.03645833333333334</v>
       </c>
       <c r="J30" t="n">
         <v>75</v>
@@ -2482,7 +2482,7 @@
         <v>27</v>
       </c>
       <c r="M30" s="1" t="n">
-        <v>0.96875</v>
+        <v>1.068965517241379</v>
       </c>
       <c r="N30" t="n">
         <v>0.003984063745019903</v>
@@ -2519,8 +2519,8 @@
       <c r="B31" t="n">
         <v>1.26965985</v>
       </c>
-      <c r="C31" s="1" t="n">
-        <v>22.64975581677708</v>
+      <c r="C31" t="n">
+        <v>18.92704318051282</v>
       </c>
       <c r="D31" t="n">
         <v>59</v>
@@ -2537,8 +2537,8 @@
       <c r="H31" t="n">
         <v>63</v>
       </c>
-      <c r="I31" s="1" t="n">
-        <v>0.01360544217687075</v>
+      <c r="I31" t="n">
+        <v>0.02083333333333333</v>
       </c>
       <c r="J31" t="n">
         <v>70</v>
@@ -2550,7 +2550,7 @@
         <v>27</v>
       </c>
       <c r="M31" s="1" t="n">
-        <v>0.9375</v>
+        <v>1.03448275862069</v>
       </c>
       <c r="N31" t="n">
         <v>0.3545816733067729</v>
@@ -2587,8 +2587,8 @@
       <c r="B32" t="n">
         <v>-0.5221736800000001</v>
       </c>
-      <c r="C32" s="1" t="n">
-        <v>21.02455583234332</v>
+      <c r="C32" t="n">
+        <v>16.50390303992081</v>
       </c>
       <c r="D32" t="n">
         <v>49</v>
@@ -2605,8 +2605,8 @@
       <c r="H32" t="n">
         <v>65</v>
       </c>
-      <c r="I32" s="1" t="n">
-        <v>0.005208333333333334</v>
+      <c r="I32" t="n">
+        <v>0.02057613168724279</v>
       </c>
       <c r="J32" t="n">
         <v>80</v>
@@ -2618,7 +2618,7 @@
         <v>24</v>
       </c>
       <c r="M32" s="1" t="n">
-        <v>0.9333333333333333</v>
+        <v>1.076923076923077</v>
       </c>
       <c r="N32" t="n">
         <v>0.4302788844621513</v>
@@ -2655,8 +2655,8 @@
       <c r="B33" t="n">
         <v>1.143782475</v>
       </c>
-      <c r="C33" s="1" t="n">
-        <v>23.46810962547405</v>
+      <c r="C33" t="n">
+        <v>19.37507748769768</v>
       </c>
       <c r="D33" t="n">
         <v>61</v>
@@ -2673,8 +2673,8 @@
       <c r="H33" t="n">
         <v>72</v>
       </c>
-      <c r="I33" s="1" t="n">
-        <v>0.01360544217687075</v>
+      <c r="I33" t="n">
+        <v>0.03645833333333334</v>
       </c>
       <c r="J33" t="n">
         <v>0</v>
@@ -2686,7 +2686,7 @@
         <v>28</v>
       </c>
       <c r="M33" s="1" t="n">
-        <v>0.9696969696969697</v>
+        <v>1.066666666666667</v>
       </c>
       <c r="N33" t="n">
         <v>0.2390438247011952</v>
@@ -2723,8 +2723,8 @@
       <c r="B34" t="n">
         <v>0.9971170300000003</v>
       </c>
-      <c r="C34" s="1" t="n">
-        <v>23.07344078445532</v>
+      <c r="C34" t="n">
+        <v>19.82103789235044</v>
       </c>
       <c r="D34" t="n">
         <v>63</v>
@@ -2741,8 +2741,8 @@
       <c r="H34" t="n">
         <v>72</v>
       </c>
-      <c r="I34" s="1" t="n">
-        <v>0.01360544217687075</v>
+      <c r="I34" t="n">
+        <v>0.03645833333333334</v>
       </c>
       <c r="J34" t="n">
         <v>0</v>
@@ -2754,7 +2754,7 @@
         <v>28</v>
       </c>
       <c r="M34" s="1" t="n">
-        <v>0.9375</v>
+        <v>1.03448275862069</v>
       </c>
       <c r="N34" t="n">
         <v>0.007968127490039823</v>
@@ -2791,8 +2791,8 @@
       <c r="B35" t="n">
         <v>0.03072110000000025</v>
       </c>
-      <c r="C35" s="1" t="n">
-        <v>18.19565705457984</v>
+      <c r="C35" t="n">
+        <v>15.01679477297077</v>
       </c>
       <c r="D35" t="n">
         <v>42</v>
@@ -2809,20 +2809,20 @@
       <c r="H35" t="n">
         <v>58</v>
       </c>
-      <c r="I35" s="1" t="n">
-        <v>0.008230452674897118</v>
+      <c r="I35" t="n">
+        <v>0.02333333333333334</v>
       </c>
       <c r="J35" t="n">
         <v>74</v>
       </c>
-      <c r="K35" s="1" t="n">
-        <v>3.320690881404089</v>
+      <c r="K35" t="n">
+        <v>3.096818523806561</v>
       </c>
       <c r="L35" t="n">
         <v>21</v>
       </c>
       <c r="M35" s="1" t="n">
-        <v>0.8518518518518519</v>
+        <v>1</v>
       </c>
       <c r="N35" t="n">
         <v>-1.734723475976807e-17</v>
@@ -2859,8 +2859,8 @@
       <c r="B36" t="n">
         <v>1.241038545</v>
       </c>
-      <c r="C36" s="1" t="n">
-        <v>23.10360836501974</v>
+      <c r="C36" t="n">
+        <v>18.95956737585637</v>
       </c>
       <c r="D36" t="n">
         <v>58</v>
@@ -2877,8 +2877,8 @@
       <c r="H36" t="n">
         <v>69</v>
       </c>
-      <c r="I36" s="1" t="n">
-        <v>0.01360544217687075</v>
+      <c r="I36" t="n">
+        <v>0.005208333333333334</v>
       </c>
       <c r="J36" t="n">
         <v>63</v>
@@ -2890,7 +2890,7 @@
         <v>27</v>
       </c>
       <c r="M36" s="1" t="n">
-        <v>1.03125</v>
+        <v>1.137931034482759</v>
       </c>
       <c r="N36" t="n">
         <v>0.3904382470119522</v>
@@ -2927,8 +2927,8 @@
       <c r="B37" t="n">
         <v>1.19502485</v>
       </c>
-      <c r="C37" s="1" t="n">
-        <v>23.22260270868652</v>
+      <c r="C37" t="n">
+        <v>19.6978788678873</v>
       </c>
       <c r="D37" t="n">
         <v>62</v>
@@ -2945,8 +2945,8 @@
       <c r="H37" t="n">
         <v>69</v>
       </c>
-      <c r="I37" s="1" t="n">
-        <v>0.01360544217687075</v>
+      <c r="I37" t="n">
+        <v>0.03645833333333334</v>
       </c>
       <c r="J37" t="n">
         <v>0</v>
@@ -2958,7 +2958,7 @@
         <v>28</v>
       </c>
       <c r="M37" s="1" t="n">
-        <v>0.9375</v>
+        <v>1</v>
       </c>
       <c r="N37" t="n">
         <v>-0.2948207171314741</v>

</xml_diff>